<commit_message>
commit de archivo xslx sobre bonos sobreanos argentinos. COMPLETO
</commit_message>
<xml_diff>
--- a/BonosARGY.xlsx
+++ b/BonosARGY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EscritorioCremona\miasaccion\Seguimiento actualizado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50718C7-C416-48C1-B4E5-E9612952A3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B7D204D-AA0E-48DC-A174-FF28EE5D4759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="747" xr2:uid="{3A827F2F-8922-486F-B015-AE1E4F07B7A5}"/>
   </bookViews>
@@ -1260,7 +1260,7 @@
     </r>
   </si>
   <si>
-    <t>https://github.com/juanupla</t>
+    <t>https://github.com/juanupla/Rendimientos-curvas_BonosSoberanos_Argentinos</t>
   </si>
 </sst>
 </file>
@@ -1853,7 +1853,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -2073,6 +2073,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8"/>
@@ -6195,7 +6196,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6227,11 +6228,17 @@
       <c r="H1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="D2" s="139" t="s">
+      <c r="A2" s="139" t="s">
         <v>211</v>
       </c>
-      <c r="E2" s="138"/>
-      <c r="H2"/>
+      <c r="B2" s="139"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="139"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="149"/>
+      <c r="I2" s="149"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D3" s="2"/>
@@ -6311,11 +6318,11 @@
       </c>
       <c r="F6" s="19">
         <f ca="1">'AL29'!$I$33</f>
-        <v>1.9666570749010655E-3</v>
+        <v>1.9932553841901599E-3</v>
       </c>
       <c r="G6" s="19">
         <f ca="1">'AL29'!I27</f>
-        <v>102.3519666570749</v>
+        <v>102.35199325538419</v>
       </c>
       <c r="H6" s="120">
         <f>'AL29'!L27</f>
@@ -6367,11 +6374,11 @@
       </c>
       <c r="F7" s="91">
         <f ca="1">'AL30'!C25</f>
-        <v>9.8332853745053276E-4</v>
+        <v>9.9662769209507996E-4</v>
       </c>
       <c r="G7" s="125">
         <f ca="1">'AL30'!C27</f>
-        <v>100.85688879147378</v>
+        <v>100.85690216451262</v>
       </c>
       <c r="H7" s="121">
         <f ca="1">'AL30'!$H$30</f>
@@ -6423,11 +6430,11 @@
       </c>
       <c r="F8" s="24">
         <f ca="1">'AL35'!J9</f>
-        <v>2.9499856123515983E-3</v>
+        <v>2.9898830762852399E-3</v>
       </c>
       <c r="G8" s="24">
         <f ca="1">'AL35'!J13</f>
-        <v>101.98294998561235</v>
+        <v>101.98298988307629</v>
       </c>
       <c r="H8" s="122">
         <f>'AL35'!J15</f>
@@ -6479,11 +6486,11 @@
       </c>
       <c r="F9" s="91">
         <f ca="1">'AE38'!K7</f>
-        <v>7.6306294506161337E-3</v>
+        <v>7.7338308906578206E-3</v>
       </c>
       <c r="G9" s="91">
         <f ca="1">'AE38'!K11</f>
-        <v>104.05763062945061</v>
+        <v>104.05773383089065</v>
       </c>
       <c r="H9" s="121">
         <f>'AE38'!K13</f>
@@ -6535,11 +6542,11 @@
       </c>
       <c r="F10" s="38">
         <f ca="1">'AL41'!J7</f>
-        <v>6.8832997621537297E-3</v>
+        <v>6.9763938446655597E-3</v>
       </c>
       <c r="G10" s="38">
         <f ca="1">'AL41'!J11</f>
-        <v>104.36688329976215</v>
+        <v>104.36697639384467</v>
       </c>
       <c r="H10" s="123">
         <f>'AL41'!J13</f>
@@ -6593,11 +6600,11 @@
       </c>
       <c r="F11" s="91">
         <f ca="1">'GD29'!J6</f>
-        <v>1.9666570749010655E-3</v>
+        <v>1.9932553841901599E-3</v>
       </c>
       <c r="G11" s="91">
         <f ca="1">'GD29'!J10</f>
-        <v>102.3519666570749</v>
+        <v>102.35199325538419</v>
       </c>
       <c r="H11" s="121">
         <f>'GD29'!J12</f>
@@ -6649,11 +6656,11 @@
       </c>
       <c r="F12" s="24">
         <f ca="1">'GD30'!J6</f>
-        <v>9.8332853745053276E-4</v>
+        <v>9.9662769209507996E-4</v>
       </c>
       <c r="G12" s="24">
         <f ca="1">'GD30'!J10</f>
-        <v>100.86098332853744</v>
+        <v>100.86099662769209</v>
       </c>
       <c r="H12" s="122">
         <f>'GD30'!J12</f>
@@ -6705,11 +6712,11 @@
       </c>
       <c r="F13" s="91">
         <f ca="1">'GD35'!J7</f>
-        <v>2.9499856123515983E-3</v>
+        <v>2.9898830762852399E-3</v>
       </c>
       <c r="G13" s="91">
         <f ca="1">'GD35'!J11</f>
-        <v>101.98294998561235</v>
+        <v>101.98298988307629</v>
       </c>
       <c r="H13" s="121">
         <f>'GD35'!J13</f>
@@ -6761,11 +6768,11 @@
       </c>
       <c r="F14" s="24">
         <f ca="1">'GD38'!L3</f>
-        <v>7.6306294506161337E-3</v>
+        <v>7.7338308906578206E-3</v>
       </c>
       <c r="G14" s="24">
         <f ca="1">'GD38'!L7</f>
-        <v>104.05763062945061</v>
+        <v>104.05773383089065</v>
       </c>
       <c r="H14" s="122">
         <f>'GD38'!L9</f>
@@ -6817,11 +6824,11 @@
       </c>
       <c r="F15" s="91">
         <f ca="1">'GD41'!J6</f>
-        <v>6.8832997621537297E-3</v>
+        <v>6.9763938446655597E-3</v>
       </c>
       <c r="G15" s="91">
         <f ca="1">'GD41'!J10</f>
-        <v>104.36688329976215</v>
+        <v>104.36697639384467</v>
       </c>
       <c r="H15" s="121">
         <f>'GD41'!J12</f>
@@ -6873,11 +6880,11 @@
       </c>
       <c r="F16" s="108">
         <f ca="1">'GD46'!J6</f>
-        <v>2.9499856123515983E-3</v>
+        <v>2.9898830762852399E-3</v>
       </c>
       <c r="G16" s="108">
         <f ca="1">'GD46'!J10</f>
-        <v>101.98294998561235</v>
+        <v>101.98298988307629</v>
       </c>
       <c r="H16" s="124">
         <f>'GD46'!J12</f>
@@ -6957,7 +6964,7 @@
       <c r="H25" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="4jnpToBZaXKqNR2ZQAbDi/3RUsDxLqmr9aYOhc/+/go4DNV8LhhcYkspGiTMa7SS0Z01QVZUvC7c+OLZqfVqoA==" saltValue="X4r+wXJmCHpAzORUiBPS6w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="uAlulCaIxpUnx/SCSM5UdLUKHCVGVjb6wyXShJDPnYvYVGTeaBt2Q9M4cANvlIlf0oz9SGEXZ+XyMqU1iM/fVQ==" saltValue="oJe6TEB+qojq7Ae9Ruj2sw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataConsolidate/>
   <mergeCells count="7">
     <mergeCell ref="L4:N4"/>
@@ -6966,10 +6973,10 @@
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="F3:H3"/>
-    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A2:E2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{20FDBD3A-0DB1-49E4-AB01-1879C681ECB8}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{2C48CD7C-1A84-4212-8CAC-20D41C6F1A09}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -7156,7 +7163,7 @@
       </c>
       <c r="J6" s="27">
         <f ca="1">IF(B4&gt;=NOW(),((NOW()-B3)/(B4-B3))*F4,IF(B5&gt;=NOW(),((NOW()-B4)/(B5-B4))*F5,IF(B6&gt;=NOW(),((NOW()-B5)/(B6-B5))*F6,IF(B7&gt;=NOW(),((NOW()-B6)/(B7-B6))*F7,IF(B8&gt;=NOW(),((NOW()-B7)/(B8-B7))*F8,IF(B9&gt;=NOW(),((NOW()-B8)/(B9-B8))*F9,IF(B10&gt;=NOW(),((NOW()-B9)/(B10-B9))*F10,IF(B11&gt;=NOW(),((NOW()-B10)/(B11-B10))*F11,IF(B12&gt;=NOW(),((NOW()-B11)/(B12-B11))*F12,IF(B13&gt;=NOW(),((NOW()-B12)/(B13-B12))*F13,IF(B14&gt;=NOW(),((NOW()-B13)/(B14-B13))*F14,IF(B15&gt;=NOW(),((NOW()-B14)/(B15-B14))*F15,IF(B16&gt;=NOW(),((NOW()-B15)/(B16-B15))*F16,IF(B17&gt;=NOW(),((NOW()-B16)/(B17-B16))*F17,IF(B18&gt;=NOW(),((NOW()-B17)/(B18-B17))*F18,IF(B19&gt;=NOW(),((NOW()-B18)/(B19-B18))*F19,IF(B20&gt;=NOW(),((NOW()-B19)/(B20-B19))*F20,IF(B21&gt;=NOW(),((NOW()-B20)/(B21-B20))*F21,IF(B22&gt;=NOW(),((NOW()-B21)/(B22-B21))*F22,"fin")))))))))))))))))))</f>
-        <v>9.8332853745053276E-4</v>
+        <v>9.9662769209507996E-4</v>
       </c>
       <c r="L6" s="22"/>
       <c r="M6">
@@ -7286,7 +7293,7 @@
       </c>
       <c r="J10" s="27">
         <f ca="1">IF(NOW()&lt;B4,C4+((NOW()-B3)/(B4-B3))*F4,IF(NOW()&lt;B5,C5+((NOW()-B4)/(B5-B4))*F5+F4,IF(NOW()&lt;B6,C6+((NOW()-B5)/(B6-B5))*F6+SUM(F4:F5),IF(NOW()&lt;B7,C7+((NOW()-B6)/(B7-B6))*F7+SUM(F4:F6),IF(NOW()&lt;B8,C8+((NOW()-B7)/(B8-B7))*F8+SUM(F4:F7),IF(NOW()&lt;B9,C9+((NOW()-B8)/(B9-B8))*F9+SUM(F4:F8),IF(NOW()&lt;B10,C10+((NOW()-B9)/(B10-B9))*F10+SUM(F4:F9),IF(NOW()&lt;B11,C11+((NOW()-B10)/(B11-B10))*F11+SUM(F4:F10),IF(NOW()&lt;B12,C12+((NOW()-B11)/(B12-B11))*F12+SUM(F4:F11),IF(NOW()&lt;B13,C13+((NOW()-B12)/(B13-B12))*F13+SUM(F4:F12),IF(NOW()&lt;B14,C14+((NOW()-B13)/(B14-B13))*F14+SUM(F4:F13),IF(NOW()&lt;B15,C15+((NOW()-B14)/(B15-B14))*F15+SUM(F4:F14),IF(NOW()&lt;B16,C16+((NOW()-B15)/(B16-B15))*F16+SUM(F4:F15),IF(NOW()&lt;B17,C17+((NOW()-B16)/(B17-B16))*F17+SUM(F4:F16),IF(NOW()&lt;B18,C18+((NOW()-B17)/(B18-B17))*F18+SUM(F4:F17),IF(NOW()&lt;B19,C19+((NOW()-B18)/(B19-B18))*F19+SUM(F4:F18),IF(NOW()&lt;B20,C20+((NOW()-B19)/(B20-B19))*F20+SUM(F4:F19),IF(NOW()&lt;B21,C21+((NOW()-B20)/(B21-B20))*F21+SUM(F4:F20),IF(NOW()&lt;B22,C22+((NOW()-B21)/(B22-B21))*F22+SUM(F4:F21),"Fin")))))))))))))))))))</f>
-        <v>100.86098332853744</v>
+        <v>100.86099662769209</v>
       </c>
       <c r="L10" s="22"/>
       <c r="M10">
@@ -7929,7 +7936,7 @@
       </c>
       <c r="J7" s="27">
         <f ca="1">IF(B4&gt;=NOW(),((NOW()-B3)/(B4-B3))*F4,IF(B5&gt;=NOW(),((NOW()-B4)/(B5-B4))*F5,IF(B6&gt;=NOW(),((NOW()-B5)/(B6-B5))*F6,IF(B7&gt;=NOW(),((NOW()-B6)/(B7-B6))*F7,IF(B8&gt;=NOW(),((NOW()-B7)/(B8-B7))*F8,IF(B9&gt;=NOW(),((NOW()-B8)/(B9-B8))*F9,IF(B10&gt;=NOW(),((NOW()-B9)/(B10-B9))*F10,IF(B11&gt;=NOW(),((NOW()-B10)/(B11-B10))*F11,IF(B12&gt;=NOW(),((NOW()-B11)/(B12-B11))*F12,IF(B13&gt;=NOW(),((NOW()-B12)/(B13-B12))*F13,IF(B14&gt;=NOW(),((NOW()-B13)/(B14-B13))*F14,IF(B15&gt;=NOW(),((NOW()-B14)/(B15-B14))*F15,IF(B16&gt;=NOW(),((NOW()-B15)/(B16-B15))*F16,IF(B17&gt;=NOW(),((NOW()-B16)/(B17-B16))*F17,IF(B18&gt;=NOW(),((NOW()-B17)/(B18-B17))*F18,IF(B19&gt;=NOW(),((NOW()-B18)/(B19-B18))*F19,IF(B20&gt;=NOW(),((NOW()-B19)/(B20-B19))*F20,IF(B21&gt;=NOW(),((NOW()-B20)/(B21-B20))*F21,IF(B22&gt;=NOW(),((NOW()-B21)/(B22-B21))*F22,IF(B23&gt;=NOW(),((NOW()-B22)/(B23-B22))*F23,IF(B24&gt;=NOW(),((NOW()-B23)/(B24-B23))*F24,IF(B25&gt;=NOW(),((NOW()-B24)/(B25-B24))*F25,IF(B26&gt;=NOW(),((NOW()-B25)/(B26-B25))*F26,IF(B27&gt;=NOW(),((NOW()-B26)/(B27-B26))*F27,IF(B28&gt;=NOW(),((NOW()-B27)/(B28-B27))*F28,IF(B29&gt;=NOW(),((NOW()-B28)/(B29-B28))*F29,IF(B30&gt;=NOW(),((NOW()-B29)/(B30-B29))*F30,IF(B31&gt;=NOW(),((NOW()-B30)/(B31-B30))*F31,IF(B32&gt;=NOW(),((NOW()-B31)/(B32-B31))*F32,"fin")))))))))))))))))))))))))))))</f>
-        <v>2.9499856123515983E-3</v>
+        <v>2.9898830762852399E-3</v>
       </c>
       <c r="L7" s="22"/>
       <c r="S7" s="12"/>
@@ -8059,7 +8066,7 @@
       </c>
       <c r="J11" s="27">
         <f ca="1">IF(NOW()&lt;B4,C4+((NOW()-B3)/(B4-B3))*F4,IF(NOW()&lt;B5,C5+((NOW()-B4)/(B5-B4))*F5+F4,IF(NOW()&lt;B6,C6+((NOW()-B5)/(B6-B5))*F6+SUM(F4:F5),IF(NOW()&lt;B7,C7+((NOW()-B6)/(B7-B6))*F7+SUM(F4:F6),IF(NOW()&lt;B8,C8+((NOW()-B7)/(B8-B7))*F8+SUM(F4:F7),IF(NOW()&lt;B9,C9+((NOW()-B8)/(B9-B8))*F9+SUM(F4:F8),IF(NOW()&lt;B10,C10+((NOW()-B9)/(B10-B9))*F10+SUM(F4:F9),IF(NOW()&lt;B11,C11+((NOW()-B10)/(B11-B10))*F11+SUM(F4:F10),IF(NOW()&lt;B12,C12+((NOW()-B11)/(B12-B11))*F12+SUM(F4:F11),IF(NOW()&lt;B13,C13+((NOW()-B12)/(B13-B12))*F13+SUM(F4:F12),IF(NOW()&lt;B14,C14+((NOW()-B13)/(B14-B13))*F14+SUM(F4:F13),IF(NOW()&lt;B15,C15+((NOW()-B14)/(B15-B14))*F15+SUM(F4:F14),IF(NOW()&lt;B16,C16+((NOW()-B15)/(B16-B15))*F16+SUM(F4:F15),IF(NOW()&lt;B17,C17+((NOW()-B16)/(B17-B16))*F17+SUM(F4:F16),IF(NOW()&lt;B18,C18+((NOW()-B17)/(B18-B17))*F18+SUM(F4:F17),IF(NOW()&lt;B19,C19+((NOW()-B18)/(B19-B18))*F19+SUM(F4:F18),IF(NOW()&lt;B20,C20+((NOW()-B19)/(B20-B19))*F20+SUM(F4:F19),IF(NOW()&lt;B21,C21+((NOW()-B20)/(B21-B20))*F21+SUM(F4:F20),IF(B22&lt;NOW(),C22+((NOW()-B21)/(B22-B21))*F22+SUM(F4:F21),IF(NOW()&lt;B23,C23+((NOW()-B22)/(B23-B22))*F23+SUM(F4:F22),IF(NOW()&lt;B24,C24+((NOW()-B23)/(B24-B23))*F24+SUM(F4:F23),IF(NOW()&lt;B25,C25+((NOW()-B24)/(B25-B24))*F25+SUM(F4:F24),IF(NOW()&lt;B26,C26+((NOW()-B25)/(B26-B25))*F26+SUM(F4:F25),IF(NOW()&lt;B27,C27+((NOW()-B26)/(B27-B26))*F27+SUM(F4:F26),IF(NOW()&lt;B28,C28+((NOW()-B27)/(B28-B27))*F28+SUM(F4:F27),IF(NOW()&lt;B29,C29+((NOW()-B28)/(B29-B28))*F29+SUM(F4:F28),IF(NOW()&lt;B30,C30+((NOW()-B29)/(B30-B29))*F30+SUM(F4:F29),IF(NOW()&lt;B31,C31+((NOW()-B30)/(B31-B30))*F31+SUM(F4:F30),IF(NOW()&lt;B32,C32+((NOW()-B31)/(B32-B31))*F32+SUM(F4:F31),"Fin")))))))))))))))))))))))))))))</f>
-        <v>101.98294998561235</v>
+        <v>101.98298988307629</v>
       </c>
       <c r="L11" s="22"/>
       <c r="S11" s="12"/>
@@ -8828,7 +8835,7 @@
       </c>
       <c r="L3" s="27">
         <f ca="1">IF(B4&gt;=NOW(),((NOW()-B3)/(B4-B3))*F4,IF(B5&gt;=NOW(),((NOW()-B4)/(B5-B4))*F5,IF(B6&gt;=NOW(),((NOW()-B5)/(B6-B5))*F6,IF(B7&gt;=NOW(),((NOW()-B6)/(B7-B6))*F7,IF(B8&gt;=NOW(),((NOW()-B7)/(B8-B7))*F8,IF(B9&gt;=NOW(),((NOW()-B8)/(B9-B8))*F9,IF(B10&gt;=NOW(),((NOW()-B9)/(B10-B9))*F10,IF(B11&gt;=NOW(),((NOW()-B10)/(B11-B10))*F11,IF(B12&gt;=NOW(),((NOW()-B11)/(B12-B11))*F12,IF(B13&gt;=NOW(),((NOW()-B12)/(B13-B12))*F13,IF(B14&gt;=NOW(),((NOW()-B13)/(B14-B13))*F14,IF(B15&gt;=NOW(),((NOW()-B14)/(B15-B14))*F15,IF(B16&gt;=NOW(),((NOW()-B15)/(B16-B15))*F16,IF(B17&gt;=NOW(),((NOW()-B16)/(B17-B16))*F17,IF(B18&gt;=NOW(),((NOW()-B17)/(B18-B17))*F18,IF(B19&gt;=NOW(),((NOW()-B18)/(B19-B18))*F19,IF(B20&gt;=NOW(),((NOW()-B19)/(B20-B19))*F20,IF(B21&gt;=NOW(),((NOW()-B20)/(B21-B20))*F21,IF(B22&gt;=NOW(),((NOW()-B21)/(B22-B21))*F22,IF(B23&gt;=NOW(),((NOW()-B22)/(B23-B22))*F23,IF(B24&gt;=NOW(),((NOW()-B23)/(B24-B23))*F24,IF(B25&gt;=NOW(),((NOW()-B24)/(B25-B24))*F25,IF(B26&gt;=NOW(),((NOW()-B25)/(B26-B25))*F26,IF(B27&gt;=NOW(),((NOW()-B26)/(B27-B26))*F27,IF(B28&gt;=NOW(),((NOW()-B27)/(B28-B27))*F28,IF(B29&gt;=NOW(),((NOW()-B28)/(B29-B28))*F29,IF(B30&gt;=NOW(),((NOW()-B29)/(B30-B29))*F30,IF(B31&gt;=NOW(),((NOW()-B30)/(B31-B30))*F31,IF(B32&gt;=NOW(),((NOW()-B31)/(B32-B31))*F32,IF(B33&gt;=NOW(),((NOW()-B32)/(B33-B32))*F33,IF(B34&gt;=NOW(),((NOW()-B33)/(B34-B33))*F34,IF(B35&gt;=NOW(),((NOW()-B34)/(B35-B34))*F35,IF(B36&gt;=NOW(),((NOW()-B35)/(B36-B35))*F36,IF(B37&gt;=NOW(),((NOW()-B36)/(B37-B36))*F37,"fin"))))))))))))))))))))))))))))))))))</f>
-        <v>7.6306294506161337E-3</v>
+        <v>7.7338308906578206E-3</v>
       </c>
       <c r="N3" s="22"/>
       <c r="U3" s="12"/>
@@ -8964,7 +8971,7 @@
       </c>
       <c r="L7" s="27">
         <f ca="1">IF(NOW()&lt;B4,C4+((NOW()-B3)/(B4-B3))*F4,IF(NOW()&lt;B5,C5+((NOW()-B4)/(B5-B4))*F5+F4,IF(NOW()&lt;B6,C6+((NOW()-B5)/(B6-B5))*F6+SUM(F4:F5),IF(NOW()&lt;B7,C7+((NOW()-B6)/(B7-B6))*F7+SUM(F4:F6),IF(NOW()&lt;B8,C8+((NOW()-B7)/(B8-B7))*F8+SUM(F4:F7),IF(NOW()&lt;B9,C9+((NOW()-B8)/(B9-B8))*F9+SUM(F4:F8),IF(NOW()&lt;B10,C10+((NOW()-B9)/(B10-B9))*F10+SUM(F4:F9),IF(NOW()&lt;B11,C11+((NOW()-B10)/(B11-B10))*F11+SUM(F4:F10),IF(NOW()&lt;B12,C12+((NOW()-B11)/(B12-B11))*F12+SUM(F4:F11),IF(NOW()&lt;B13,C13+((NOW()-B12)/(B13-B12))*F13+SUM(F4:F12),IF(NOW()&lt;B14,C14+((NOW()-B13)/(B14-B13))*F14+SUM(F4:F13),IF(NOW()&lt;B15,C15+((NOW()-B14)/(B15-B14))*F15+SUM(F4:F14),IF(NOW()&lt;B16,C16+((NOW()-B15)/(B16-B15))*F16+SUM(F4:F15),IF(NOW()&lt;B17,C17+((NOW()-B16)/(B17-B16))*F17+SUM(F4:F16),IF(NOW()&lt;B18,C18+((NOW()-B17)/(B18-B17))*F18+SUM(F4:F17),IF(NOW()&lt;B19,C19+((NOW()-B18)/(B19-B18))*F19+SUM(F4:F18),IF(NOW()&lt;B20,C20+((NOW()-B19)/(B20-B19))*F20+SUM(F4:F19),IF(NOW()&lt;B21,C21+((NOW()-B20)/(B21-B20))*F21+SUM(F4:F20),IF(B22&lt;NOW(),C22+((NOW()-B21)/(B22-B21))*F22+SUM(F4:F21),IF(NOW()&lt;B23,C23+((NOW()-B22)/(B23-B22))*F23+SUM(F4:F22),IF(NOW()&lt;B24,C24+((NOW()-B23)/(B24-B23))*F24+SUM(F4:F23),IF(NOW()&lt;B25,C25+((NOW()-B24)/(B25-B24))*F25+SUM(F4:F24),IF(NOW()&lt;B26,C26+((NOW()-B25)/(B26-B25))*F26+SUM(F4:F25),IF(NOW()&lt;B27,C27+((NOW()-B26)/(B27-B26))*F27+SUM(F4:F26),IF(NOW()&lt;B28,C28+((NOW()-B27)/(B28-B27))*F28+SUM(F4:F27),IF(NOW()&lt;B29,C29+((NOW()-B28)/(B29-B28))*F29+SUM(F4:F28),IF(NOW()&lt;B30,C30+((NOW()-B29)/(B30-B29))*F30+SUM(F4:F29),IF(NOW()&lt;B31,C31+((NOW()-B30)/(B31-B30))*F31+SUM(F4:F30),IF(NOW()&lt;B32,C32+((NOW()-B31)/(B32-B31))*F32+SUM(F4:F31),IF(NOW()&lt;B33,C33+((NOW()-B32)/(B33-B32))*F33+SUM(F4:F32),IF(NOW()&lt;B34,C34+((NOW()-B33)/(B34-B33))*F34+SUM(F4:F33),IF(NOW()&lt;B35,C35+((NOW()-B34)/(B35-B34))*F35+SUM(F4:F34),IF(NOW()&lt;B36,C36+((NOW()-B35)/(B36-B35))*F36+SUM(F4:F35),IF(NOW()&lt;B37,C37+((NOW()-B36)/(B37-B36))*F37+SUM(F4:F36),"fin"))))))))))))))))))))))))))))))))))</f>
-        <v>104.05763062945061</v>
+        <v>104.05773383089065</v>
       </c>
       <c r="N7" s="22"/>
       <c r="U7" s="12"/>
@@ -10092,7 +10099,7 @@
       </c>
       <c r="J6" s="27">
         <f ca="1">IF(B4&gt;=NOW(),((NOW()-B3)/(B4-B3))*F4,IF(B5&gt;=NOW(),((NOW()-B4)/(B5-B4))*F5,IF(B6&gt;=NOW(),((NOW()-B5)/(B6-B5))*F6,IF(B7&gt;=NOW(),((NOW()-B6)/(B7-B6))*F7,IF(B8&gt;=NOW(),((NOW()-B7)/(B8-B7))*F8,IF(B9&gt;=NOW(),((NOW()-B8)/(B9-B8))*F9,IF(B10&gt;=NOW(),((NOW()-B9)/(B10-B9))*F10,IF(B11&gt;=NOW(),((NOW()-B10)/(B11-B10))*F11,IF(B12&gt;=NOW(),((NOW()-B11)/(B12-B11))*F12,IF(B13&gt;=NOW(),((NOW()-B12)/(B13-B12))*F13,IF(B14&gt;=NOW(),((NOW()-B13)/(B14-B13))*F14,IF(B15&gt;=NOW(),((NOW()-B14)/(B15-B14))*F15,IF(B16&gt;=NOW(),((NOW()-B15)/(B16-B15))*F16,IF(B17&gt;=NOW(),((NOW()-B16)/(B17-B16))*F17,IF(B18&gt;=NOW(),((NOW()-B17)/(B18-B17))*F18,IF(B19&gt;=NOW(),((NOW()-B18)/(B19-B18))*F19,IF(B20&gt;=NOW(),((NOW()-B19)/(B20-B19))*F20,IF(B21&gt;=NOW(),((NOW()-B20)/(B21-B20))*F21,IF(B22&gt;=NOW(),((NOW()-B21)/(B22-B21))*F22,IF(B23&gt;=NOW(),((NOW()-B22)/(B23-B22))*F23,IF(B24&gt;=NOW(),((NOW()-B23)/(B24-B23))*F24,IF(B25&gt;=NOW(),((NOW()-B24)/(B25-B24))*F25,IF(B26&gt;=NOW(),((NOW()-B25)/(B26-B25))*F26,IF(B27&gt;=NOW(),((NOW()-B26)/(B27-B26))*F27,IF(B28&gt;=NOW(),((NOW()-B27)/(B28-B27))*F28,IF(B29&gt;=NOW(),((NOW()-B28)/(B29-B28))*F29,IF(B30&gt;=NOW(),((NOW()-B29)/(B30-B29))*F30,IF(B31&gt;=NOW(),((NOW()-B30)/(B31-B30))*F31,IF(B32&gt;=NOW(),((NOW()-B31)/(B32-B31))*F32,IF(B33&gt;=NOW(),((NOW()-B32)/(B33-B32))*F33,IF(B34&gt;=NOW(),((NOW()-B33)/(B34-B33))*F34,IF(B35&gt;=NOW(),((NOW()-B34)/(B35-B34))*F35,IF(B36&gt;=NOW(),((NOW()-B35)/(B36-B35))*F36,IF(B37&gt;=NOW(),((NOW()-B36)/(B37-B36))*F37,IF(B38&gt;=NOW(),((NOW()-B37)/(B38-B37))*F38,IF(B39&gt;=NOW(),((NOW()-B38)/(B39-B38))*F39,IF(B40&gt;=NOW(),((NOW()-B39)/(B40-B39))*F40,IF(B41&gt;=NOW(),((NOW()-B40)/(B41-B40))*F41,IF(B42&gt;=NOW(),((NOW()-B41)/(B42-B41))*F42,IF(B43&gt;=NOW(),((NOW()-B42)/(B43-B42))*F43,IF(B44&gt;=NOW(),((NOW()-B43)/(B44-B43))*F44,"fin")))))))))))))))))))))))))))))))))))))))))</f>
-        <v>6.8832997621537297E-3</v>
+        <v>6.9763938446655597E-3</v>
       </c>
       <c r="L6" s="22"/>
       <c r="M6">
@@ -10222,7 +10229,7 @@
       </c>
       <c r="J10" s="27">
         <f ca="1">IF(NOW()&lt;B4,C4+((NOW()-B3)/(B4-B3))*F4,IF(NOW()&lt;B5,C5+((NOW()-B4)/(B5-B4))*F5+F4,IF(NOW()&lt;B6,C6+((NOW()-B5)/(B6-B5))*F6+SUM(F4:F5),IF(NOW()&lt;B7,C7+((NOW()-B6)/(B7-B6))*F7+SUM(F4:F6),IF(NOW()&lt;B8,C8+((NOW()-B7)/(B8-B7))*F8+SUM(F4:F7),IF(NOW()&lt;B9,C9+((NOW()-B8)/(B9-B8))*F9+SUM(F4:F8),IF(NOW()&lt;B10,C10+((NOW()-B9)/(B10-B9))*F10+SUM(F4:F9),IF(NOW()&lt;B11,C11+((NOW()-B10)/(B11-B10))*F11+SUM(F4:F10),IF(NOW()&lt;B12,C12+((NOW()-B11)/(B12-B11))*F12+SUM(F4:F11),IF(NOW()&lt;B13,C13+((NOW()-B12)/(B13-B12))*F13+SUM(F4:F12),IF(NOW()&lt;B14,C14+((NOW()-B13)/(B14-B13))*F14+SUM(F4:F13),IF(NOW()&lt;B15,C15+((NOW()-B14)/(B15-B14))*F15+SUM(F4:F14),IF(NOW()&lt;B16,C16+((NOW()-B15)/(B16-B15))*F16+SUM(F4:F15),IF(NOW()&lt;B17,C17+((NOW()-B16)/(B17-B16))*F17+SUM(F4:F16),IF(NOW()&lt;B18,C18+((NOW()-B17)/(B18-B17))*F18+SUM(F4:F17),IF(NOW()&lt;B19,C19+((NOW()-B18)/(B19-B18))*F19+SUM(F4:F18),IF(NOW()&lt;B20,C20+((NOW()-B19)/(B20-B19))*F20+SUM(F4:F19),IF(NOW()&lt;B21,C21+((NOW()-B20)/(B21-B20))*F21+SUM(F4:F20),IF(B22&lt;NOW(),C22+((NOW()-B21)/(B22-B21))*F22+SUM(F4:F21),IF(NOW()&lt;B23,C23+((NOW()-B22)/(B23-B22))*F23+SUM(F4:F22),IF(NOW()&lt;B24,C24+((NOW()-B23)/(B24-B23))*F24+SUM(F4:F23),IF(NOW()&lt;B25,C25+((NOW()-B24)/(B25-B24))*F25+SUM(F4:F24),IF(NOW()&lt;B26,C26+((NOW()-B25)/(B26-B25))*F26+SUM(F4:F25),IF(NOW()&lt;B27,C27+((NOW()-B26)/(B27-B26))*F27+SUM(F4:F26),IF(NOW()&lt;B28,C28+((NOW()-B27)/(B28-B27))*F28+SUM(F4:F27),IF(NOW()&lt;B29,C29+((NOW()-B28)/(B29-B28))*F29+SUM(F4:F28),IF(NOW()&lt;B30,C30+((NOW()-B29)/(B30-B29))*F30+SUM(F4:F29),IF(NOW()&lt;B31,C31+((NOW()-B30)/(B31-B30))*F31+SUM(F4:F30),IF(NOW()&lt;B32,C32+((NOW()-B31)/(B32-B31))*F32+SUM(F4:F31),IF(NOW()&lt;B33,C33+((NOW()-B32)/(B33-B32))*F33+SUM(F4:F32),IF(NOW()&lt;B34,C34+((NOW()-B33)/(B34-B33))*F34+SUM(F4:F33),IF(B35&lt;NOW(),C35+((NOW()-B34)/(B35-B34))*F35+SUM(F4:F34),IF(NOW()&lt;B36,C36+((NOW()-B35)/(B36-B35))*F36+SUM(F4:F35),IF(NOW()&lt;B37,C37+((NOW()-B36)/(B37-B36))*F37+SUM(F4:F36),IF(NOW()&lt;B38,C38+((NOW()-B37)/(B38-B37))*F38+SUM(F4:F37),IF(NOW()&lt;B39,C39+((NOW()-B38)/(B39-B38))*F39+SUM(F4:F38),IF(NOW()&lt;B40,C40+((NOW()-B39)/(B40-B39))*F40+SUM(F4:F39),IF(NOW()&lt;B41,C41+((NOW()-B40)/(B41-B40))*F41+SUM(F4:F40),IF(NOW()&lt;B42,C42+((NOW()-B41)/(B42-B41))*F42+SUM(F4:F41),IF(NOW()&lt;B43,C43+((NOW()-B42)/(B43-B42))*F43+SUM(F4:F42),IF(NOW()&lt;B44,C44+((NOW()-B43)/(B44-B43))*F44+SUM(F4:F43),"Fin")))))))))))))))))))))))))))))))))))))))))</f>
-        <v>104.36688329976215</v>
+        <v>104.36697639384467</v>
       </c>
       <c r="L10" s="22"/>
       <c r="M10">
@@ -11473,7 +11480,7 @@
       </c>
       <c r="J6" s="27">
         <f ca="1">IF(B4&gt;=NOW(),((NOW()-B3)/(B4-B3))*F4,IF(B5&gt;=NOW(),((NOW()-B4)/(B5-B4))*F5,IF(B6&gt;=NOW(),((NOW()-B5)/(B6-B5))*F6,IF(B7&gt;=NOW(),((NOW()-B6)/(B7-B6))*F7,IF(B8&gt;=NOW(),((NOW()-B7)/(B8-B7))*F8,IF(B9&gt;=NOW(),((NOW()-B8)/(B9-B8))*F9,IF(B10&gt;=NOW(),((NOW()-B9)/(B10-B9))*F10,IF(B11&gt;=NOW(),((NOW()-B10)/(B11-B10))*F11,IF(B12&gt;=NOW(),((NOW()-B11)/(B12-B11))*F12,IF(B13&gt;=NOW(),((NOW()-B12)/(B13-B12))*F13,IF(B14&gt;=NOW(),((NOW()-B13)/(B14-B13))*F14,IF(B15&gt;=NOW(),((NOW()-B14)/(B15-B14))*F15,IF(B16&gt;=NOW(),((NOW()-B15)/(B16-B15))*F16,IF(B17&gt;=NOW(),((NOW()-B16)/(B17-B16))*F17,IF(B18&gt;=NOW(),((NOW()-B17)/(B18-B17))*F18,IF(B19&gt;=NOW(),((NOW()-B18)/(B19-B18))*F19,IF(B20&gt;=NOW(),((NOW()-B19)/(B20-B19))*F20,IF(B21&gt;=NOW(),((NOW()-B20)/(B21-B20))*F21,IF(B22&gt;=NOW(),((NOW()-B21)/(B22-B21))*F22,IF(B23&gt;=NOW(),((NOW()-B22)/(B23-B22))*F23,IF(B24&gt;=NOW(),((NOW()-B23)/(B24-B23))*F24,IF(B25&gt;=NOW(),((NOW()-B24)/(B25-B24))*F25,IF(B26&gt;=NOW(),((NOW()-B25)/(B26-B25))*F26,IF(B27&gt;=NOW(),((NOW()-B26)/(B27-B26))*F27,IF(B28&gt;=NOW(),((NOW()-B27)/(B28-B27))*F28,IF(B29&gt;=NOW(),((NOW()-B28)/(B29-B28))*F29,IF(B30&gt;=NOW(),((NOW()-B29)/(B30-B29))*F30,IF(B31&gt;=NOW(),((NOW()-B30)/(B31-B30))*F31,IF(B32&gt;=NOW(),((NOW()-B31)/(B32-B31))*F32,IF(B33&gt;=NOW(),((NOW()-B32)/(B33-B32))*F33,IF(B34&gt;=NOW(),((NOW()-B33)/(B34-B33))*F34,IF(B35&gt;=NOW(),((NOW()-B34)/(B35-B34))*F35,IF(B36&gt;=NOW(),((NOW()-B35)/(B36-B35))*F36,IF(B37&gt;=NOW(),((NOW()-B36)/(B37-B36))*F37,IF(B38&gt;=NOW(),((NOW()-B37)/(B38-B37))*F38,IF(B39&gt;=NOW(),((NOW()-B38)/(B39-B38))*F39,IF(B40&gt;=NOW(),((NOW()-B39)/(B40-B39))*F40,IF(B41&gt;=NOW(),((NOW()-B40)/(B41-B40))*F41,IF(B42&gt;=NOW(),((NOW()-B41)/(B42-B41))*F42,IF(B43&gt;=NOW(),((NOW()-B42)/(B43-B42))*F43,IF(B44&gt;=NOW(),((NOW()-B43)/(B44-B43))*F44,IF(B45&gt;=NOW(),((NOW()-B44)/(B45-B44))*F45,IF(B46&gt;=NOW(),((NOW()-B45)/(B46-B45))*F46,IF(B47&gt;=NOW(),((NOW()-B46)/(B47-B46))*F47,IF(B48&gt;=NOW(),((NOW()-B47)/(B48-B47))*F48,IF(B49&gt;=NOW(),((NOW()-B48)/(B49-B48))*F49,IF(B50&gt;=NOW(),((NOW()-B49)/(B50-B49))*F50,IF(B51&gt;=NOW(),((NOW()-B50)/(B51-B50))*F51,IF(B52&gt;=NOW(),((NOW()-B51)/(B52-B51))*F52,IF(B53&gt;=NOW(),((NOW()-B52)/(B53-B52))*F53,IF(B54&gt;=NOW(),((NOW()-B53)/(B54-B53))*F54,"fin")))))))))))))))))))))))))))))))))))))))))))))))))))</f>
-        <v>2.9499856123515983E-3</v>
+        <v>2.9898830762852399E-3</v>
       </c>
       <c r="L6" s="22"/>
       <c r="M6">
@@ -11603,7 +11610,7 @@
       </c>
       <c r="J10" s="27">
         <f ca="1">IF(NOW()&lt;B4,C4+((NOW()-B3)/(B4-B3))*F4,IF(NOW()&lt;B5,C5+((NOW()-B4)/(B5-B4))*F5+F4,IF(NOW()&lt;B6,C6+((NOW()-B5)/(B6-B5))*F6+SUM(F4:F5),IF(NOW()&lt;B7,C7+((NOW()-B6)/(B7-B6))*F7+SUM(F4:F6),IF(NOW()&lt;B8,C8+((NOW()-B7)/(B8-B7))*F8+SUM(F4:F7),IF(NOW()&lt;B9,C9+((NOW()-B8)/(B9-B8))*F9+SUM(F4:F8),IF(NOW()&lt;B10,C10+((NOW()-B9)/(B10-B9))*F10+SUM(F4:F9),IF(NOW()&lt;B11,C11+((NOW()-B10)/(B11-B10))*F11+SUM(F4:F10),IF(NOW()&lt;B12,C12+((NOW()-B11)/(B12-B11))*F12+SUM(F4:F11),IF(NOW()&lt;B13,C13+((NOW()-B12)/(B13-B12))*F13+SUM(F4:F12),IF(NOW()&lt;B14,C14+((NOW()-B13)/(B14-B13))*F14+SUM(F4:F13),IF(NOW()&lt;B15,C15+((NOW()-B14)/(B15-B14))*F15+SUM(F4:F14),IF(NOW()&lt;B16,C16+((NOW()-B15)/(B16-B15))*F16+SUM(F4:F15),IF(NOW()&lt;B17,C17+((NOW()-B16)/(B17-B16))*F17+SUM(F4:F16),IF(NOW()&lt;B18,C18+((NOW()-B17)/(B18-B17))*F18+SUM(F4:F17),IF(NOW()&lt;B19,C19+((NOW()-B18)/(B19-B18))*F19+SUM(F4:F18),IF(NOW()&lt;B20,C20+((NOW()-B19)/(B20-B19))*F20+SUM(F4:F19),IF(NOW()&lt;B21,C21+((NOW()-B20)/(B21-B20))*F21+SUM(F4:F20),IF(B22&lt;NOW(),C22+((NOW()-B21)/(B22-B21))*F22+SUM(F4:F21),IF(NOW()&lt;B23,C23+((NOW()-B22)/(B23-B22))*F23+SUM(F4:F22),IF(NOW()&lt;B24,C24+((NOW()-B23)/(B24-B23))*F24+SUM(F4:F23),IF(NOW()&lt;B25,C25+((NOW()-B24)/(B25-B24))*F25+SUM(F4:F24),IF(NOW()&lt;B26,C26+((NOW()-B25)/(B26-B25))*F26+SUM(F4:F25),IF(NOW()&lt;B27,C27+((NOW()-B26)/(B27-B26))*F27+SUM(F4:F26),IF(NOW()&lt;B28,C28+((NOW()-B27)/(B28-B27))*F28+SUM(F4:F27),IF(NOW()&lt;B29,C29+((NOW()-B28)/(B29-B28))*F29+SUM(F4:F28),IF(NOW()&lt;B30,C30+((NOW()-B29)/(B30-B29))*F30+SUM(F4:F29),IF(NOW()&lt;B31,C31+((NOW()-B30)/(B31-B30))*F31+SUM(F4:F30),IF(NOW()&lt;B32,C32+((NOW()-B31)/(B32-B31))*F32+SUM(F4:F31),IF(NOW()&lt;B33,C33+((NOW()-B32)/(B33-B32))*F33+SUM(F4:F32),IF(NOW()&lt;B34,C34+((NOW()-B33)/(B34-B33))*F34+SUM(F4:F33),IF(B35&lt;NOW(),C35+((NOW()-B34)/(B35-B34))*F35+SUM(F4:F34),IF(NOW()&lt;B36,C36+((NOW()-B35)/(B36-B35))*F36+SUM(F4:F35),IF(NOW()&lt;B37,C37+((NOW()-B36)/(B37-B36))*F37+SUM(F4:F36),IF(NOW()&lt;B38,C38+((NOW()-B37)/(B38-B37))*F38+SUM(F4:F37),IF(NOW()&lt;B39,C39+((NOW()-B38)/(B39-B38))*F39+SUM(F4:F38),IF(NOW()&lt;B40,C40+((NOW()-B39)/(B40-B39))*F40+SUM(F4:F39),IF(NOW()&lt;B41,C41+((NOW()-B40)/(B41-B40))*F41+SUM(F4:F40),IF(NOW()&lt;B42,C42+((NOW()-B41)/(B42-B41))*F42+SUM(F4:F41),IF(NOW()&lt;B43,C43+((NOW()-B42)/(B43-B42))*F43+SUM(F4:F42),IF(NOW()&lt;B44,C44+((NOW()-B43)/(B44-B43))*F44+SUM(F4:F43),IF(NOW()&lt;B45,C45+((NOW()-B44)/(B45-B44))*F45+SUM(F4:F44),IF(NOW()&lt;B46,C46+((NOW()-B45)/(B46-B45))*F46+SUM(F4:F45),IF(NOW()&lt;B47,C47+((NOW()-B46)/(B47-B46))*F47+SUM(F4:F46),IF(NOW()&lt;B48,C48+((NOW()-B47)/(B48-B47))*F48+SUM(F4:F47),IF(NOW()&lt;B49,C49+((NOW()-B48)/(B49-B48))*F49+SUM(F4:F48),IF(NOW()&lt;B50,C50+((NOW()-B49)/(B50-B49))*F50+SUM(F4:F49),IF(NOW()&lt;B51,C51+((NOW()-B50)/(B51-B50))*F51+SUM(F4:F50),IF(NOW()&lt;B52,C52+((NOW()-B51)/(B52-B51))*F52+SUM(F4:F51),IF(NOW()&lt;B53,C53+((NOW()-B52)/(B53-B52))*F53+SUM(F4:F52),IF(NOW()&lt;B54,C54+((NOW()-B53)/(B54-B53))*F54+SUM(F4:F53),"Fin")))))))))))))))))))))))))))))))))))))))))))))))))))</f>
-        <v>101.98294998561235</v>
+        <v>101.98298988307629</v>
       </c>
       <c r="L10" s="22"/>
       <c r="M10">
@@ -13362,8 +13369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7A4057-4F86-422D-8D01-7E2251D0D8EE}">
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A98"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13453,10 +13460,10 @@
         <v>114</v>
       </c>
       <c r="B3" s="127">
-        <v>10511</v>
+        <v>10515</v>
       </c>
       <c r="C3" s="11">
-        <v>-2.3999999999999998E-3</v>
+        <v>-2E-3</v>
       </c>
       <c r="D3" t="s">
         <v>101</v>
@@ -13480,7 +13487,7 @@
         <v>10537</v>
       </c>
       <c r="K3" s="127">
-        <v>269770307.19</v>
+        <v>278838967.87</v>
       </c>
       <c r="L3" s="11">
         <v>0</v>
@@ -13535,10 +13542,10 @@
         <v>116</v>
       </c>
       <c r="B5">
-        <v>32.299999999999997</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="C5" s="11">
-        <v>1.5699999999999999E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="D5" t="s">
         <v>101</v>
@@ -13562,7 +13569,7 @@
         <v>31.8</v>
       </c>
       <c r="K5" s="127">
-        <v>58384.44</v>
+        <v>64655.32</v>
       </c>
       <c r="L5" s="11">
         <v>0</v>
@@ -13576,10 +13583,10 @@
         <v>117</v>
       </c>
       <c r="B6" s="127">
-        <v>9025</v>
+        <v>9050</v>
       </c>
       <c r="C6" s="11">
-        <v>1.12E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="D6" t="s">
         <v>101</v>
@@ -13603,7 +13610,7 @@
         <v>8925</v>
       </c>
       <c r="K6" s="127">
-        <v>18069180</v>
+        <v>20587123.879999999</v>
       </c>
       <c r="L6" s="11">
         <v>0</v>
@@ -13658,10 +13665,10 @@
         <v>119</v>
       </c>
       <c r="B8">
-        <v>27.65</v>
+        <v>27.8</v>
       </c>
       <c r="C8" s="11">
-        <v>3.1699999999999999E-2</v>
+        <v>3.73E-2</v>
       </c>
       <c r="D8" t="s">
         <v>101</v>
@@ -13685,7 +13692,7 @@
         <v>26.8</v>
       </c>
       <c r="K8" s="127">
-        <v>34277.160000000003</v>
+        <v>42050.12</v>
       </c>
       <c r="L8" s="11">
         <v>0</v>
@@ -13699,10 +13706,10 @@
         <v>120</v>
       </c>
       <c r="B9" s="127">
-        <v>8676.5</v>
+        <v>8670</v>
       </c>
       <c r="C9" s="11">
-        <v>2.3699999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="D9" t="s">
         <v>101</v>
@@ -13726,7 +13733,7 @@
         <v>8475</v>
       </c>
       <c r="K9" s="127">
-        <v>2215541388.0100002</v>
+        <v>2451713621.0900002</v>
       </c>
       <c r="L9" s="11">
         <v>0</v>
@@ -13781,10 +13788,10 @@
         <v>122</v>
       </c>
       <c r="B11">
-        <v>26.55</v>
+        <v>26.5</v>
       </c>
       <c r="C11" s="11">
-        <v>3.7999999999999999E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="D11" t="s">
         <v>101</v>
@@ -13808,7 +13815,7 @@
         <v>25.58</v>
       </c>
       <c r="K11" s="127">
-        <v>1594114.38</v>
+        <v>1935326.93</v>
       </c>
       <c r="L11" s="11">
         <v>0</v>
@@ -13822,10 +13829,10 @@
         <v>123</v>
       </c>
       <c r="B12" s="127">
-        <v>8960</v>
+        <v>8966</v>
       </c>
       <c r="C12" s="11">
-        <v>7.6E-3</v>
+        <v>8.3000000000000001E-3</v>
       </c>
       <c r="D12" t="s">
         <v>101</v>
@@ -13849,7 +13856,7 @@
         <v>8892</v>
       </c>
       <c r="K12" s="127">
-        <v>47992433.829999998</v>
+        <v>49851662.630000003</v>
       </c>
       <c r="L12" s="11">
         <v>0</v>
@@ -13904,10 +13911,10 @@
         <v>125</v>
       </c>
       <c r="B14">
-        <v>27.47</v>
+        <v>27.5</v>
       </c>
       <c r="C14" s="11">
-        <v>2.8799999999999999E-2</v>
+        <v>2.9899999999999999E-2</v>
       </c>
       <c r="D14" t="s">
         <v>101</v>
@@ -13931,7 +13938,7 @@
         <v>26.7</v>
       </c>
       <c r="K14" s="127">
-        <v>9788.1</v>
+        <v>17303.07</v>
       </c>
       <c r="L14" s="11">
         <v>0</v>
@@ -13945,10 +13952,10 @@
         <v>126</v>
       </c>
       <c r="B15" s="127">
-        <v>9735</v>
+        <v>9650</v>
       </c>
       <c r="C15" s="11">
-        <v>-1.5E-3</v>
+        <v>-1.0200000000000001E-2</v>
       </c>
       <c r="D15" t="s">
         <v>101</v>
@@ -13972,7 +13979,7 @@
         <v>9750</v>
       </c>
       <c r="K15" s="127">
-        <v>124445395.73999999</v>
+        <v>129238609.02</v>
       </c>
       <c r="L15" s="11">
         <v>0</v>
@@ -14027,10 +14034,10 @@
         <v>128</v>
       </c>
       <c r="B17">
-        <v>30</v>
+        <v>29.9</v>
       </c>
       <c r="C17" s="4">
-        <v>0</v>
+        <v>-3.3E-3</v>
       </c>
       <c r="D17" t="s">
         <v>101</v>
@@ -14109,10 +14116,10 @@
         <v>130</v>
       </c>
       <c r="B19" s="127">
-        <v>13500</v>
+        <v>13749</v>
       </c>
       <c r="C19" s="11">
-        <v>3.0499999999999999E-2</v>
+        <v>4.9500000000000002E-2</v>
       </c>
       <c r="D19" t="s">
         <v>101</v>
@@ -14136,7 +14143,7 @@
         <v>13100</v>
       </c>
       <c r="K19" s="127">
-        <v>3818960.97</v>
+        <v>4460210.97</v>
       </c>
       <c r="L19" s="11">
         <v>0</v>
@@ -14232,10 +14239,10 @@
         <v>133</v>
       </c>
       <c r="B22">
-        <v>34.200000000000003</v>
+        <v>34</v>
       </c>
       <c r="C22" s="11">
-        <v>5.7999999999999996E-3</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>101</v>
@@ -14396,10 +14403,10 @@
         <v>137</v>
       </c>
       <c r="B26">
-        <v>103.6</v>
+        <v>104.5</v>
       </c>
       <c r="C26" s="11">
-        <v>-1.9E-3</v>
+        <v>6.7000000000000002E-3</v>
       </c>
       <c r="D26" t="s">
         <v>101</v>
@@ -14423,7 +14430,7 @@
         <v>103.8</v>
       </c>
       <c r="K26" s="127">
-        <v>3926028.9</v>
+        <v>4106171.69</v>
       </c>
       <c r="L26" s="11">
         <v>0</v>
@@ -14437,10 +14444,10 @@
         <v>138</v>
       </c>
       <c r="B27">
-        <v>106.45</v>
+        <v>106.35</v>
       </c>
       <c r="C27" s="11">
-        <v>4.1999999999999997E-3</v>
+        <v>3.3E-3</v>
       </c>
       <c r="D27" t="s">
         <v>101</v>
@@ -14464,7 +14471,7 @@
         <v>106</v>
       </c>
       <c r="K27" s="127">
-        <v>1985849.71</v>
+        <v>1987549.45</v>
       </c>
       <c r="L27" s="11">
         <v>0</v>
@@ -14587,7 +14594,7 @@
         <v>17949</v>
       </c>
       <c r="K30" s="127">
-        <v>78553119.319999993</v>
+        <v>80628129.319999993</v>
       </c>
       <c r="L30" s="11">
         <v>-6.8900000000000003E-2</v>
@@ -14642,10 +14649,10 @@
         <v>143</v>
       </c>
       <c r="B32" s="127">
-        <v>2680</v>
+        <v>2670</v>
       </c>
       <c r="C32" s="11">
-        <v>-7.7000000000000002E-3</v>
+        <v>-1.14E-2</v>
       </c>
       <c r="D32" t="s">
         <v>101</v>
@@ -14669,7 +14676,7 @@
         <v>2701</v>
       </c>
       <c r="K32" s="127">
-        <v>614377.27</v>
+        <v>1027532.18</v>
       </c>
       <c r="L32" s="11">
         <v>4.1700000000000001E-2</v>
@@ -14683,10 +14690,10 @@
         <v>144</v>
       </c>
       <c r="B33" s="127">
-        <v>4975</v>
+        <v>4980</v>
       </c>
       <c r="C33" s="11">
-        <v>-1.8E-3</v>
+        <v>-8.0000000000000004E-4</v>
       </c>
       <c r="D33" t="s">
         <v>101</v>
@@ -14710,7 +14717,7 @@
         <v>4984</v>
       </c>
       <c r="K33" s="127">
-        <v>12476405.24</v>
+        <v>12972468.390000001</v>
       </c>
       <c r="L33" s="11">
         <v>-5.1000000000000004E-3</v>
@@ -14765,10 +14772,10 @@
         <v>146</v>
       </c>
       <c r="B35" s="127">
-        <v>9697</v>
+        <v>9898</v>
       </c>
       <c r="C35" s="11">
-        <v>4.7999999999999996E-3</v>
+        <v>2.5600000000000001E-2</v>
       </c>
       <c r="D35" t="s">
         <v>101</v>
@@ -14792,7 +14799,7 @@
         <v>9650</v>
       </c>
       <c r="K35" s="127">
-        <v>4185774.85</v>
+        <v>4202938.54</v>
       </c>
       <c r="L35" s="11">
         <v>0</v>
@@ -14888,10 +14895,10 @@
         <v>149</v>
       </c>
       <c r="B38" s="127">
-        <v>9930</v>
+        <v>9915</v>
       </c>
       <c r="C38" s="11">
-        <v>1.4800000000000001E-2</v>
+        <v>1.32E-2</v>
       </c>
       <c r="D38" t="s">
         <v>101</v>
@@ -14915,7 +14922,7 @@
         <v>9785</v>
       </c>
       <c r="K38" s="127">
-        <v>5183874755.8599997</v>
+        <v>5579867062.5299997</v>
       </c>
       <c r="L38" s="11">
         <v>0</v>
@@ -14956,7 +14963,7 @@
         <v>29.25</v>
       </c>
       <c r="K39" s="127">
-        <v>153806.21</v>
+        <v>261487.89</v>
       </c>
       <c r="L39" s="11">
         <v>0</v>
@@ -14970,10 +14977,10 @@
         <v>151</v>
       </c>
       <c r="B40">
-        <v>30.33</v>
+        <v>30.35</v>
       </c>
       <c r="C40" s="11">
-        <v>2.2599999999999999E-2</v>
+        <v>2.3199999999999998E-2</v>
       </c>
       <c r="D40" t="s">
         <v>101</v>
@@ -14997,7 +15004,7 @@
         <v>29.66</v>
       </c>
       <c r="K40" s="127">
-        <v>8348599.5099999998</v>
+        <v>9609233.1999999993</v>
       </c>
       <c r="L40" s="11">
         <v>0</v>
@@ -15011,10 +15018,10 @@
         <v>152</v>
       </c>
       <c r="B41" s="127">
-        <v>9330</v>
+        <v>9290</v>
       </c>
       <c r="C41" s="11">
-        <v>1.9599999999999999E-2</v>
+        <v>1.5299999999999999E-2</v>
       </c>
       <c r="D41" t="s">
         <v>101</v>
@@ -15038,7 +15045,7 @@
         <v>9150</v>
       </c>
       <c r="K41" s="127">
-        <v>160425182.33000001</v>
+        <v>171645273.31999999</v>
       </c>
       <c r="L41" s="11">
         <v>0</v>
@@ -15093,10 +15100,10 @@
         <v>154</v>
       </c>
       <c r="B43">
-        <v>28.54</v>
+        <v>28.52</v>
       </c>
       <c r="C43" s="11">
-        <v>2.07E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D43" t="s">
         <v>101</v>
@@ -15120,7 +15127,7 @@
         <v>27.96</v>
       </c>
       <c r="K43" s="127">
-        <v>26484.13</v>
+        <v>33306.33</v>
       </c>
       <c r="L43" s="11">
         <v>0</v>
@@ -15134,10 +15141,10 @@
         <v>155</v>
       </c>
       <c r="B44" s="127">
-        <v>11350</v>
+        <v>11440</v>
       </c>
       <c r="C44" s="11">
-        <v>4.8999999999999998E-3</v>
+        <v>1.29E-2</v>
       </c>
       <c r="D44" t="s">
         <v>101</v>
@@ -15161,7 +15168,7 @@
         <v>11294</v>
       </c>
       <c r="K44" s="127">
-        <v>110565482.19</v>
+        <v>127096743.98999999</v>
       </c>
       <c r="L44" s="11">
         <v>0</v>
@@ -15257,10 +15264,10 @@
         <v>158</v>
       </c>
       <c r="B47" s="127">
-        <v>10419</v>
+        <v>10595</v>
       </c>
       <c r="C47" s="11">
-        <v>8.0999999999999996E-3</v>
+        <v>2.5100000000000001E-2</v>
       </c>
       <c r="D47" t="s">
         <v>101</v>
@@ -15284,7 +15291,7 @@
         <v>10335</v>
       </c>
       <c r="K47" s="127">
-        <v>286927365.58999997</v>
+        <v>288163348.54000002</v>
       </c>
       <c r="L47" s="11">
         <v>0</v>
@@ -15380,10 +15387,10 @@
         <v>161</v>
       </c>
       <c r="B50" s="127">
-        <v>9550</v>
+        <v>9900</v>
       </c>
       <c r="C50" s="11">
-        <v>5.1999999999999998E-3</v>
+        <v>4.2099999999999999E-2</v>
       </c>
       <c r="D50" t="s">
         <v>101</v>
@@ -15407,7 +15414,7 @@
         <v>9500</v>
       </c>
       <c r="K50" s="127">
-        <v>2319529.15</v>
+        <v>2406682.65</v>
       </c>
       <c r="L50" s="11">
         <v>0</v>
@@ -15544,10 +15551,10 @@
         <v>165</v>
       </c>
       <c r="B54" s="127">
-        <v>2090</v>
+        <v>2080</v>
       </c>
       <c r="C54" s="11">
-        <v>-2.06E-2</v>
+        <v>-2.53E-2</v>
       </c>
       <c r="D54" t="s">
         <v>101</v>
@@ -15571,7 +15578,7 @@
         <v>2134</v>
       </c>
       <c r="K54" s="127">
-        <v>13045161.609999999</v>
+        <v>13114843.210000001</v>
       </c>
       <c r="L54" s="11">
         <v>2.86E-2</v>
@@ -15585,10 +15592,10 @@
         <v>166</v>
       </c>
       <c r="B55">
-        <v>107.45</v>
+        <v>107.4</v>
       </c>
       <c r="C55" s="11">
-        <v>1.2999999999999999E-3</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="D55" t="s">
         <v>101</v>
@@ -15612,7 +15619,7 @@
         <v>107.3</v>
       </c>
       <c r="K55" s="127">
-        <v>20455771.5</v>
+        <v>24964928.5</v>
       </c>
       <c r="L55" s="11">
         <v>0</v>
@@ -15708,10 +15715,10 @@
         <v>169</v>
       </c>
       <c r="B58" s="127">
-        <v>27000</v>
+        <v>26800</v>
       </c>
       <c r="C58" s="11">
-        <v>7.4000000000000003E-3</v>
+        <v>0</v>
       </c>
       <c r="D58" t="s">
         <v>101</v>
@@ -15790,10 +15797,10 @@
         <v>171</v>
       </c>
       <c r="B60">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="C60" s="11">
-        <v>-3.7000000000000002E-3</v>
+        <v>-1.1999999999999999E-3</v>
       </c>
       <c r="D60" t="s">
         <v>101</v>
@@ -15817,7 +15824,7 @@
         <v>803</v>
       </c>
       <c r="K60" s="127">
-        <v>875191.72</v>
+        <v>887191.72</v>
       </c>
       <c r="L60" s="11">
         <v>-0.2306</v>
@@ -16077,10 +16084,10 @@
         <v>178</v>
       </c>
       <c r="B67" s="127">
-        <v>17825</v>
+        <v>17850</v>
       </c>
       <c r="C67" s="11">
-        <v>-5.3E-3</v>
+        <v>-3.8999999999999998E-3</v>
       </c>
       <c r="D67" t="s">
         <v>101</v>
@@ -16104,7 +16111,7 @@
         <v>17920</v>
       </c>
       <c r="K67" s="127">
-        <v>2496504.65</v>
+        <v>3387754.65</v>
       </c>
       <c r="L67" s="11">
         <v>0</v>
@@ -16186,7 +16193,7 @@
         <v>321</v>
       </c>
       <c r="K69" s="127">
-        <v>88388567.260000005</v>
+        <v>88596191.810000002</v>
       </c>
       <c r="L69" s="11">
         <v>0</v>
@@ -16200,10 +16207,10 @@
         <v>181</v>
       </c>
       <c r="B70">
-        <v>234.75</v>
+        <v>234.55</v>
       </c>
       <c r="C70" s="11">
-        <v>3.2000000000000002E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="D70" t="s">
         <v>101</v>
@@ -16227,7 +16234,7 @@
         <v>234</v>
       </c>
       <c r="K70" s="127">
-        <v>17402439.670000002</v>
+        <v>17551728.399999999</v>
       </c>
       <c r="L70" s="11">
         <v>0</v>
@@ -16241,10 +16248,10 @@
         <v>182</v>
       </c>
       <c r="B71">
-        <v>112.4</v>
+        <v>113</v>
       </c>
       <c r="C71" s="11">
-        <v>2.5999999999999999E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D71" t="s">
         <v>101</v>
@@ -16268,7 +16275,7 @@
         <v>112.1</v>
       </c>
       <c r="K71" s="127">
-        <v>72327.42</v>
+        <v>75494.23</v>
       </c>
       <c r="L71" s="11">
         <v>0</v>
@@ -16364,10 +16371,10 @@
         <v>185</v>
       </c>
       <c r="B74">
-        <v>660.2</v>
+        <v>660</v>
       </c>
       <c r="C74" s="4">
-        <v>0</v>
+        <v>-2.9999999999999997E-4</v>
       </c>
       <c r="D74" t="s">
         <v>101</v>
@@ -16391,7 +16398,7 @@
         <v>660.2</v>
       </c>
       <c r="K74" s="127">
-        <v>1219178.1599999999</v>
+        <v>1224016.56</v>
       </c>
       <c r="L74" s="11">
         <v>0</v>
@@ -16432,7 +16439,7 @@
         <v>16500</v>
       </c>
       <c r="K75" s="127">
-        <v>235707158.34</v>
+        <v>253681792.34</v>
       </c>
       <c r="L75" s="11">
         <v>0</v>
@@ -16528,10 +16535,10 @@
         <v>189</v>
       </c>
       <c r="B78" s="127">
-        <v>17860</v>
+        <v>17880</v>
       </c>
       <c r="C78" s="11">
-        <v>-6.8999999999999999E-3</v>
+        <v>-5.7999999999999996E-3</v>
       </c>
       <c r="D78" t="s">
         <v>101</v>
@@ -16555,7 +16562,7 @@
         <v>17985</v>
       </c>
       <c r="K78" s="127">
-        <v>65557542.689999998</v>
+        <v>77575308.290000007</v>
       </c>
       <c r="L78" s="11">
         <v>0</v>
@@ -16610,10 +16617,10 @@
         <v>191</v>
       </c>
       <c r="B80" s="127">
-        <v>17755</v>
+        <v>17770</v>
       </c>
       <c r="C80" s="11">
-        <v>-5.0000000000000001E-3</v>
+        <v>-4.1999999999999997E-3</v>
       </c>
       <c r="D80" t="s">
         <v>101</v>
@@ -16637,7 +16644,7 @@
         <v>17845</v>
       </c>
       <c r="K80" s="127">
-        <v>29716236.199999999</v>
+        <v>31930107.149999999</v>
       </c>
       <c r="L80" s="11">
         <v>0</v>
@@ -16651,10 +16658,10 @@
         <v>192</v>
       </c>
       <c r="B81" s="127">
-        <v>17389</v>
+        <v>17250</v>
       </c>
       <c r="C81" s="11">
-        <v>-5.1999999999999998E-3</v>
+        <v>-1.3100000000000001E-2</v>
       </c>
       <c r="D81" t="s">
         <v>101</v>
@@ -16678,7 +16685,7 @@
         <v>17480</v>
       </c>
       <c r="K81" s="127">
-        <v>15504573.529999999</v>
+        <v>16308293.33</v>
       </c>
       <c r="L81" s="11">
         <v>0</v>
@@ -16774,10 +16781,10 @@
         <v>195</v>
       </c>
       <c r="B84">
-        <v>68.849999999999994</v>
+        <v>68.900000000000006</v>
       </c>
       <c r="C84" s="11">
-        <v>4.8999999999999998E-3</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="D84" t="s">
         <v>101</v>
@@ -16801,7 +16808,7 @@
         <v>68.510000000000005</v>
       </c>
       <c r="K84" s="127">
-        <v>24761308.800000001</v>
+        <v>25004906.66</v>
       </c>
       <c r="L84" s="11">
         <v>0.50680000000000003</v>
@@ -16815,10 +16822,10 @@
         <v>196</v>
       </c>
       <c r="B85">
-        <v>28.5</v>
+        <v>28.69</v>
       </c>
       <c r="C85" s="4">
-        <v>0</v>
+        <v>6.6E-3</v>
       </c>
       <c r="D85" t="s">
         <v>101</v>
@@ -16833,7 +16840,7 @@
         <v>101</v>
       </c>
       <c r="H85">
-        <v>28.5</v>
+        <v>28.7</v>
       </c>
       <c r="I85">
         <v>27.9</v>
@@ -16842,7 +16849,7 @@
         <v>28.5</v>
       </c>
       <c r="K85" s="127">
-        <v>5121868.37</v>
+        <v>5655852.6600000001</v>
       </c>
       <c r="L85" s="11">
         <v>0.48080000000000001</v>
@@ -16856,10 +16863,10 @@
         <v>197</v>
       </c>
       <c r="B86" s="127">
-        <v>17715</v>
+        <v>17725</v>
       </c>
       <c r="C86" s="11">
-        <v>-5.0000000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="D86" t="s">
         <v>101</v>
@@ -16883,7 +16890,7 @@
         <v>17725</v>
       </c>
       <c r="K86" s="127">
-        <v>1004743632.26</v>
+        <v>1334008192.76</v>
       </c>
       <c r="L86" s="11">
         <v>0</v>
@@ -16924,7 +16931,7 @@
         <v>15270</v>
       </c>
       <c r="K87" s="127">
-        <v>58856446.799999997</v>
+        <v>70003196.299999997</v>
       </c>
       <c r="L87" s="11">
         <v>0</v>
@@ -17020,10 +17027,10 @@
         <v>201</v>
       </c>
       <c r="B90">
-        <v>1.36</v>
+        <v>1.4</v>
       </c>
       <c r="C90" s="11">
-        <v>-2.8500000000000001E-2</v>
+        <v>-6.9999999999999999E-4</v>
       </c>
       <c r="D90" t="s">
         <v>101</v>
@@ -17041,13 +17048,13 @@
         <v>1.47</v>
       </c>
       <c r="I90">
-        <v>1.34</v>
+        <v>1</v>
       </c>
       <c r="J90">
         <v>1.4</v>
       </c>
       <c r="K90" s="127">
-        <v>397352.28</v>
+        <v>959315.74</v>
       </c>
       <c r="L90" s="11">
         <v>0</v>
@@ -17143,10 +17150,10 @@
         <v>204</v>
       </c>
       <c r="B93">
-        <v>359.35</v>
+        <v>359.6</v>
       </c>
       <c r="C93" s="11">
-        <v>-4.0000000000000002E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="D93" t="s">
         <v>101</v>
@@ -17170,7 +17177,7 @@
         <v>359.5</v>
       </c>
       <c r="K93" s="127">
-        <v>50231522.789999999</v>
+        <v>57228406.880000003</v>
       </c>
       <c r="L93" s="11">
         <v>0</v>
@@ -17211,7 +17218,7 @@
         <v>325.3</v>
       </c>
       <c r="K94" s="127">
-        <v>339534073.13999999</v>
+        <v>342530127.16000003</v>
       </c>
       <c r="L94" s="11">
         <v>0</v>
@@ -17266,10 +17273,10 @@
         <v>207</v>
       </c>
       <c r="B96">
-        <v>242.5</v>
+        <v>242.45</v>
       </c>
       <c r="C96" s="11">
-        <v>-5.1000000000000004E-3</v>
+        <v>-5.3E-3</v>
       </c>
       <c r="D96" t="s">
         <v>101</v>
@@ -17293,7 +17300,7 @@
         <v>243.75</v>
       </c>
       <c r="K96" s="127">
-        <v>27888599.390000001</v>
+        <v>30390245.870000001</v>
       </c>
       <c r="L96" s="11">
         <v>0</v>
@@ -17307,10 +17314,10 @@
         <v>208</v>
       </c>
       <c r="B97">
-        <v>232</v>
+        <v>234.4</v>
       </c>
       <c r="C97" s="11">
-        <v>-1.23E-2</v>
+        <v>-2.0999999999999999E-3</v>
       </c>
       <c r="D97" t="s">
         <v>101</v>
@@ -17334,7 +17341,7 @@
         <v>234.9</v>
       </c>
       <c r="K97" s="127">
-        <v>5910557.9900000002</v>
+        <v>7787463.9000000004</v>
       </c>
       <c r="L97" s="11">
         <v>0</v>
@@ -17385,7 +17392,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="sxKu+/i/SuBznJVn3ziqt0DRfjGdGxBYFDQrsGD9n8PgryYKCDpdm5bBIaCqaR6IwApUv9Icbq7TLTpYV1naEw==" saltValue="VQMMjJghHM9a7IGK8nStjQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -18055,7 +18062,7 @@
       </c>
       <c r="I27" s="28">
         <f ca="1">IF(NOW()&lt;B4,C4+((NOW()-B3)/(B4-B3))*F4,IF(NOW()&lt;B5,C5+((NOW()-B4)/(B5-B4))*F5+F4,IF(NOW()&lt;B6,C6+((NOW()-B5)/(B6-B5))*F6+SUM(F4:F5),IF(NOW()&lt;B7,C7+((NOW()-B6)/(B7-B6))*F7+SUM(F4:F6),IF(NOW()&lt;B8,C8+((NOW()-B7)/(B8-B7))*F8+SUM(F4:F7),IF(NOW()&lt;B9,C9+((NOW()-B8)/(B9-B8))*F9+SUM(F4:F8),IF(NOW()&lt;B10,C10+((NOW()-B9)/(B10-B9))*F10+SUM(F4:F9),IF(NOW()&lt;B11,C11+((NOW()-B10)/(B11-B10))*F11+SUM(F4:F10),IF(NOW()&lt;B12,C12+((NOW()-B11)/(B12-B11))*F12+SUM(F4:F11),IF(NOW()&lt;B13,C13+((NOW()-B12)/(B13-B12))*F13+SUM(F4:F12),IF(NOW()&lt;B14,C14+((NOW()-B13)/(B14-B13))*F14+SUM(F4:F13),IF(NOW()&lt;B15,C15+((NOW()-B14)/(B15-B14))*F15+SUM(F4:F14),IF(NOW()&lt;B16,C16+((NOW()-B15)/(B16-B15))*F16+SUM(F4:F15),IF(NOW()&lt;B17,C17+((NOW()-B16)/(B17-B16))*F17+SUM(F4:F16),IF(NOW()&lt;B18,C18+((NOW()-B17)/(B18-B17))*F18+SUM(F4:F17),IF(NOW()&lt;B19,C19+((NOW()-B18)/(B19-B18))*F19+SUM(F4:F18),IF(NOW()&lt;B20,C20+((NOW()-B19)/(B20-B19))*F20+SUM(F4:F19),"fin")))))))))))))))))</f>
-        <v>102.3519666570749</v>
+        <v>102.35199325538419</v>
       </c>
       <c r="K27" s="27" t="s">
         <v>40</v>
@@ -18140,7 +18147,7 @@
       </c>
       <c r="I33" s="28">
         <f ca="1">IF(B4&gt;=NOW(),((NOW()-B3)/(B4-B3))*F4,IF(B5&gt;=NOW(),((NOW()-B4)/(B5-B4))*F5,IF(B6&gt;=NOW(),((NOW()-B5)/(B6-B5))*F6,IF(B7&gt;=NOW(),((NOW()-B6)/(B7-B6))*F7,IF(B8&gt;=NOW(),((NOW()-B7)/(B8-B7))*F8,IF(B9&gt;=NOW(),((NOW()-B8)/(B9-B8))*F9,IF(B10&gt;=NOW(),((NOW()-B9)/(B10-B9))*F10,IF(B11&gt;=NOW(),((NOW()-B10)/(B11-B10))*F11,IF(B12&gt;=NOW(),((NOW()-B11)/(B12-B11))*F12,IF(B13&gt;=NOW(),((NOW()-B12)/(B13-B12))*F13,IF(B14&gt;=NOW(),((NOW()-B13)/(B14-B13))*F14,IF(B15&gt;=NOW(),((NOW()-B14)/(B15-B14))*F15,IF(B16&gt;=NOW(),((NOW()-B15)/(B16-B15))*F16,IF(B17&gt;=NOW(),((NOW()-B16)/(B17-B16))*F17,IF(B18&gt;=NOW(),((NOW()-B17)/(B18-B17))*F18,IF(B19&gt;=NOW(),((NOW()-B18)/(B19-B18))*F19,IF(B20&gt;=NOW(),((NOW()-B19)/(B20-B19))*F20,"fin")))))))))))))))))</f>
-        <v>1.9666570749010655E-3</v>
+        <v>1.9932553841901599E-3</v>
       </c>
       <c r="L33" s="11"/>
       <c r="P33" s="138" t="s">
@@ -18234,7 +18241,7 @@
       </c>
       <c r="I3" s="1">
         <f ca="1">NOW()</f>
-        <v>44935.711929861114</v>
+        <v>44935.721558449077</v>
       </c>
       <c r="J3" t="s">
         <v>8</v>
@@ -18972,7 +18979,7 @@
       </c>
       <c r="C25" s="34">
         <f ca="1">IF(C4&gt;=NOW(),((NOW()-C3)/(C4-C3))*F4,IF(C5&gt;=NOW(),((NOW()-C4)/(C5-C4))*F5,IF(C6&gt;=NOW(),((NOW()-C5)/(C6-C5))*F6,IF(C7&gt;=NOW(),((NOW()-C6)/(C7-C6))*F7,IF(C8&gt;=NOW(),((NOW()-C7)/(C8-C7))*F8,IF(C9&gt;=NOW(),((NOW()-C8)/(C9-C8))*F9,IF(C10&gt;=NOW(),((NOW()-C9)/(C10-C9))*F10,IF(C11&gt;=NOW(),((NOW()-C10)/(C11-C10))*F11,IF(C12&gt;=NOW(),((NOW()-C11)/(C12-C11))*F12,IF(C13&gt;=NOW(),((NOW()-C12)/(C13-C12))*F13,IF(C14&gt;=NOW(),((NOW()-C13)/(C14-C13))*F14,IF(C15&gt;=NOW(),((NOW()-C14)/(C15-C14))*F15,IF(C16&gt;=NOW(),((NOW()-C15)/(C16-C15))*F16,IF(C17&gt;=NOW(),((NOW()-C16)/(C17-C16))*F17,IF(C18&gt;=NOW(),((NOW()-C17)/(C18-C17))*F18,IF(C19&gt;=NOW(),((NOW()-C18)/(C19-C18))*F19,IF(C20&gt;=NOW(),((NOW()-C19)/(C20-C19))*F20,IF(C21&gt;=NOW(),((NOW()-C20)/(C21-C20))*F21,IF(C22&gt;=NOW(),((NOW()-C21)/(C22-C21))*F22,"fin")))))))))))))))))))</f>
-        <v>9.8332853745053276E-4</v>
+        <v>9.9662769209507996E-4</v>
       </c>
       <c r="E25" s="27" t="s">
         <v>19</v>
@@ -18991,7 +18998,7 @@
       </c>
       <c r="C27" s="28">
         <f ca="1">IF(NOW()&lt;C4,D4+((NOW()-C3)/300)*F4,IF(NOW()&lt;C5,D5+((NOW()-C4)/180)*F5+F4,IF(NOW()&lt;C6,D6+((NOW()-C5)/180)*F6+SUM(F4:F5),IF(NOW()&lt;C7,D7+((NOW()-C6)/180)*F7+SUM(F4:F6),IF(NOW()&lt;C8,D8+((NOW()-C7)/180)*F8+SUM(F4:F7),IF(NOW()&lt;C9,D9+((NOW()-C8)/180)*F9+SUM(F4:F8),IF(NOW()&lt;C10,D10+((NOW()-C9)/180)*F10+SUM(F4:F9),IF(NOW()&lt;C11,D11+((NOW()-C10)/180)*F11+SUM(F4:F10),IF(NOW()&lt;C12,D12+((NOW()-C11)/180)*F12+SUM(F4:F11),IF(NOW()&lt;C13,D13+((NOW()-C12)/180)*F13+SUM(F4:F12),IF(NOW()&lt;C14,D14+((NOW()-C13)/180)*F14+SUM(F4:F13),IF(NOW()&lt;C15,D15+((NOW()-C14)/180)*F15+SUM(F4:F14),IF(NOW()&lt;C16,D16+((NOW()-C15)/180)*F16+SUM(F4:F15),IF(NOW()&lt;C17,D17+((NOW()-C16)/180)*F17+SUM(F4:F16),IF(NOW()&lt;C18,D18+((NOW()-C17)/180)*F18+SUM(F4:F17),IF(NOW()&lt;C19,D19+((NOW()-C18)/180)*F19+SUM(F4:F18),IF(NOW()&lt;C20,D20+((NOW()-C19)/180)*F20+SUM(F4:F19),IF(NOW()&lt;C21,D21+((NOW()-C20)/180)*F21+SUM(F4:F20),IF(NOW()&lt;C22,D22+((NOW()-C21)/180)*F22+SUM(F4:F21),"fin")))))))))))))))))))</f>
-        <v>100.85688879147378</v>
+        <v>100.85690216451262</v>
       </c>
       <c r="E27" s="1"/>
     </row>
@@ -19347,7 +19354,7 @@
       </c>
       <c r="J9" s="27">
         <f ca="1">IF(B4&gt;=NOW(),((NOW()-B3)/(B4-B3))*F4,IF(B5&gt;=NOW(),((NOW()-B4)/(B5-B4))*F5,IF(B6&gt;=NOW(),((NOW()-B5)/(B6-B5))*F6,IF(B7&gt;=NOW(),((NOW()-B6)/(B7-B6))*F7,IF(B8&gt;=NOW(),((NOW()-B7)/(B8-B7))*F8,IF(B9&gt;=NOW(),((NOW()-B8)/(B9-B8))*F9,IF(B10&gt;=NOW(),((NOW()-B9)/(B10-B9))*F10,IF(B11&gt;=NOW(),((NOW()-B10)/(B11-B10))*F11,IF(B12&gt;=NOW(),((NOW()-B11)/(B12-B11))*F12,IF(B13&gt;=NOW(),((NOW()-B12)/(B13-B12))*F13,IF(B14&gt;=NOW(),((NOW()-B13)/(B14-B13))*F14,IF(B15&gt;=NOW(),((NOW()-B14)/(B15-B14))*F15,IF(B16&gt;=NOW(),((NOW()-B15)/(B16-B15))*F16,IF(B17&gt;=NOW(),((NOW()-B16)/(B17-B16))*F17,IF(B18&gt;=NOW(),((NOW()-B17)/(B18-B17))*F18,IF(B19&gt;=NOW(),((NOW()-B18)/(B19-B18))*F19,IF(B20&gt;=NOW(),((NOW()-B19)/(B20-B19))*F20,IF(B21&gt;=NOW(),((NOW()-B20)/(B21-B20))*F21,IF(B22&gt;=NOW(),((NOW()-B21)/(B22-B21))*F22,IF(B23&gt;=NOW(),((NOW()-B22)/(B23-B22))*F23,IF(B24&gt;=NOW(),((NOW()-B23)/(B24-B23))*F24,IF(B25&gt;=NOW(),((NOW()-B24)/(B25-B24))*F25,IF(B26&gt;=NOW(),((NOW()-B25)/(B26-B25))*F26,IF(B27&gt;=NOW(),((NOW()-B26)/(B27-B26))*F27,IF(B28&gt;=NOW(),((NOW()-B27)/(B28-B27))*F28,IF(B29&gt;=NOW(),((NOW()-B28)/(B29-B28))*F29,IF(B30&gt;=NOW(),((NOW()-B29)/(B30-B29))*F30,IF(B31&gt;=NOW(),((NOW()-B30)/(B31-B30))*F31,IF(B32&gt;=NOW(),((NOW()-B31)/(B32-B31))*F32,"fin")))))))))))))))))))))))))))))</f>
-        <v>2.9499856123515983E-3</v>
+        <v>2.9898830762852399E-3</v>
       </c>
       <c r="M9" s="22"/>
       <c r="T9" s="12"/>
@@ -19477,7 +19484,7 @@
       </c>
       <c r="J13" s="27">
         <f ca="1">IF(NOW()&lt;B4,C4+((NOW()-B3)/(B4-B3))*F4,IF(NOW()&lt;B5,C5+((NOW()-B4)/(B5-B4))*F5+F4,IF(NOW()&lt;B6,C6+((NOW()-B5)/(B6-B5))*F6+SUM(F4:F5),IF(NOW()&lt;B7,C7+((NOW()-B6)/(B7-B6))*F7+SUM(F4:F6),IF(NOW()&lt;B8,C8+((NOW()-B7)/(B8-B7))*F8+SUM(F4:F7),IF(NOW()&lt;B9,C9+((NOW()-B8)/(B9-B8))*F9+SUM(F4:F8),IF(NOW()&lt;B10,C10+((NOW()-B9)/(B10-B9))*F10+SUM(F4:F9),IF(NOW()&lt;B11,C11+((NOW()-B10)/(B11-B10))*F11+SUM(F4:F10),IF(NOW()&lt;B12,C12+((NOW()-B11)/(B12-B11))*F12+SUM(F4:F11),IF(NOW()&lt;B13,C13+((NOW()-B12)/(B13-B12))*F13+SUM(F4:F12),IF(NOW()&lt;B14,C14+((NOW()-B13)/(B14-B13))*F14+SUM(F4:F13),IF(NOW()&lt;B15,C15+((NOW()-B14)/(B15-B14))*F15+SUM(F4:F14),IF(NOW()&lt;B16,C16+((NOW()-B15)/(B16-B15))*F16+SUM(F4:F15),IF(NOW()&lt;B17,C17+((NOW()-B16)/(B17-B16))*F17+SUM(F4:F16),IF(NOW()&lt;B18,C18+((NOW()-B17)/(B18-B17))*F18+SUM(F4:F17),IF(NOW()&lt;B19,C19+((NOW()-B18)/(B19-B18))*F19+SUM(F4:F18),IF(NOW()&lt;B20,C20+((NOW()-B19)/(B20-B19))*F20+SUM(F4:F19),IF(NOW()&lt;B21,C21+((NOW()-B20)/(B21-B20))*F21+SUM(F4:F20),IF(B22&lt;NOW(),C22+((NOW()-B21)/(B22-B21))*F22+SUM(F4:F21),IF(NOW()&lt;B23,C23+((NOW()-B22)/(B23-B22))*F23+SUM(F4:F22),IF(NOW()&lt;B24,C24+((NOW()-B23)/(B24-B23))*F24+SUM(F4:F23),IF(NOW()&lt;B25,C25+((NOW()-B24)/(B25-B24))*F25+SUM(F4:F24),IF(NOW()&lt;B26,C26+((NOW()-B25)/(B26-B25))*F26+SUM(F4:F25),IF(NOW()&lt;B27,C27+((NOW()-B26)/(B27-B26))*F27+SUM(F4:F26),IF(NOW()&lt;B28,C28+((NOW()-B27)/(B28-B27))*F28+SUM(F4:F27),IF(NOW()&lt;B29,C29+((NOW()-B28)/(B29-B28))*F29+SUM(F4:F28),IF(NOW()&lt;B30,C30+((NOW()-B29)/(B30-B29))*F30+SUM(F4:F29),IF(NOW()&lt;B31,C31+((NOW()-B30)/(B31-B30))*F31+SUM(F4:F30),IF(NOW()&lt;B32,C32+((NOW()-B31)/(B32-B31))*F32+SUM(F4:F31),"Fin")))))))))))))))))))))))))))))</f>
-        <v>101.98294998561235</v>
+        <v>101.98298988307629</v>
       </c>
       <c r="M13" s="22"/>
       <c r="T13" s="12"/>
@@ -20317,7 +20324,7 @@
       </c>
       <c r="K7">
         <f ca="1">IF(B4&gt;=NOW(),((NOW()-B3)/(B4-B3))*F4,IF(B5&gt;=NOW(),((NOW()-B4)/(B5-B4))*F5,IF(B6&gt;=NOW(),((NOW()-B5)/(B6-B5))*F6,IF(B7&gt;=NOW(),((NOW()-B6)/(B7-B6))*F7,IF(B8&gt;=NOW(),((NOW()-B7)/(B8-B7))*F8,IF(B9&gt;=NOW(),((NOW()-B8)/(B9-B8))*F9,IF(B10&gt;=NOW(),((NOW()-B9)/(B10-B9))*F10,IF(B11&gt;=NOW(),((NOW()-B10)/(B11-B10))*F11,IF(B12&gt;=NOW(),((NOW()-B11)/(B12-B11))*F12,IF(B13&gt;=NOW(),((NOW()-B12)/(B13-B12))*F13,IF(B14&gt;=NOW(),((NOW()-B13)/(B14-B13))*F14,IF(B15&gt;=NOW(),((NOW()-B14)/(B15-B14))*F15,IF(B16&gt;=NOW(),((NOW()-B15)/(B16-B15))*F16,IF(B17&gt;=NOW(),((NOW()-B16)/(B17-B16))*F17,IF(B18&gt;=NOW(),((NOW()-B17)/(B18-B17))*F18,IF(B19&gt;=NOW(),((NOW()-B18)/(B19-B18))*F19,IF(B20&gt;=NOW(),((NOW()-B19)/(B20-B19))*F20,IF(B21&gt;=NOW(),((NOW()-B20)/(B21-B20))*F21,IF(B22&gt;=NOW(),((NOW()-B21)/(B22-B21))*F22,IF(B23&gt;=NOW(),((NOW()-B22)/(B23-B22))*F23,IF(B24&gt;=NOW(),((NOW()-B23)/(B24-B23))*F24,IF(B25&gt;=NOW(),((NOW()-B24)/(B25-B24))*F25,IF(B26&gt;=NOW(),((NOW()-B25)/(B26-B25))*F26,IF(B27&gt;=NOW(),((NOW()-B26)/(B27-B26))*F27,IF(B28&gt;=NOW(),((NOW()-B27)/(B28-B27))*F28,IF(B29&gt;=NOW(),((NOW()-B28)/(B29-B28))*F29,IF(B30&gt;=NOW(),((NOW()-B29)/(B30-B29))*F30,IF(B31&gt;=NOW(),((NOW()-B30)/(B31-B30))*F31,IF(B32&gt;=NOW(),((NOW()-B31)/(B32-B31))*F32,IF(B33&gt;=NOW(),((NOW()-B32)/(B33-B32))*F33,IF(B34&gt;=NOW(),((NOW()-B33)/(B34-B33))*F34,IF(B35&gt;=NOW(),((NOW()-B34)/(B35-B34))*F35,IF(B36&gt;=NOW(),((NOW()-B35)/(B36-B35))*F36,IF(B37&gt;=NOW(),((NOW()-B36)/(B37-B36))*F37,"fin"))))))))))))))))))))))))))))))))))</f>
-        <v>7.6306294506161337E-3</v>
+        <v>7.7338308906578206E-3</v>
       </c>
       <c r="M7" s="22"/>
       <c r="T7" s="12"/>
@@ -20447,7 +20454,7 @@
       </c>
       <c r="K11">
         <f ca="1">IF(NOW()&lt;B4,C4+((NOW()-B3)/(B4-B3))*F4,IF(NOW()&lt;B5,C5+((NOW()-B4)/(B5-B4))*F5+F4,IF(NOW()&lt;B6,C6+((NOW()-B5)/(B6-B5))*F6+SUM(F4:F5),IF(NOW()&lt;B7,C7+((NOW()-B6)/(B7-B6))*F7+SUM(F4:F6),IF(NOW()&lt;B8,C8+((NOW()-B7)/(B8-B7))*F8+SUM(F4:F7),IF(NOW()&lt;B9,C9+((NOW()-B8)/(B9-B8))*F9+SUM(F4:F8),IF(NOW()&lt;B10,C10+((NOW()-B9)/(B10-B9))*F10+SUM(F4:F9),IF(NOW()&lt;B11,C11+((NOW()-B10)/(B11-B10))*F11+SUM(F4:F10),IF(NOW()&lt;B12,C12+((NOW()-B11)/(B12-B11))*F12+SUM(F4:F11),IF(NOW()&lt;B13,C13+((NOW()-B12)/(B13-B12))*F13+SUM(F4:F12),IF(NOW()&lt;B14,C14+((NOW()-B13)/(B14-B13))*F14+SUM(F4:F13),IF(NOW()&lt;B15,C15+((NOW()-B14)/(B15-B14))*F15+SUM(F4:F14),IF(NOW()&lt;B16,C16+((NOW()-B15)/(B16-B15))*F16+SUM(F4:F15),IF(NOW()&lt;B17,C17+((NOW()-B16)/(B17-B16))*F17+SUM(F4:F16),IF(NOW()&lt;B18,C18+((NOW()-B17)/(B18-B17))*F18+SUM(F4:F17),IF(NOW()&lt;B19,C19+((NOW()-B18)/(B19-B18))*F19+SUM(F4:F18),IF(NOW()&lt;B20,C20+((NOW()-B19)/(B20-B19))*F20+SUM(F4:F19),IF(NOW()&lt;B21,C21+((NOW()-B20)/(B21-B20))*F21+SUM(F4:F20),IF(B22&lt;NOW(),C22+((NOW()-B21)/(B22-B21))*F22+SUM(F4:F21),IF(NOW()&lt;B23,C23+((NOW()-B22)/(B23-B22))*F23+SUM(F4:F22),IF(NOW()&lt;B24,C24+((NOW()-B23)/(B24-B23))*F24+SUM(F4:F23),IF(NOW()&lt;B25,C25+((NOW()-B24)/(B25-B24))*F25+SUM(F4:F24),IF(NOW()&lt;B26,C26+((NOW()-B25)/(B26-B25))*F26+SUM(F4:F25),IF(NOW()&lt;B27,C27+((NOW()-B26)/(B27-B26))*F27+SUM(F4:F26),IF(NOW()&lt;B28,C28+((NOW()-B27)/(B28-B27))*F28+SUM(F4:F27),IF(NOW()&lt;B29,C29+((NOW()-B28)/(B29-B28))*F29+SUM(F4:F28),IF(NOW()&lt;B30,C30+((NOW()-B29)/(B30-B29))*F30+SUM(F4:F29),IF(NOW()&lt;B31,C31+((NOW()-B30)/(B31-B30))*F31+SUM(F4:F30),IF(NOW()&lt;B32,C32+((NOW()-B31)/(B32-B31))*F32+SUM(F4:F31),IF(NOW()&lt;B33,C33+((NOW()-B32)/(B33-B32))*F33+SUM(F4:F32),IF(NOW()&lt;B34,C34+((NOW()-B33)/(B34-B33))*F34+SUM(F4:F33),IF(NOW()&lt;B35,C35+((NOW()-B34)/(B35-B34))*F35+SUM(F4:F34),IF(NOW()&lt;B36,C36+((NOW()-B35)/(B36-B35))*F36+SUM(F4:F35),IF(NOW()&lt;B37,C37+((NOW()-B36)/(B37-B36))*F37+SUM(F4:F36),"fin"))))))))))))))))))))))))))))))))))</f>
-        <v>104.05763062945061</v>
+        <v>104.05773383089065</v>
       </c>
       <c r="M11" s="22"/>
       <c r="T11" s="12"/>
@@ -21501,7 +21508,7 @@
       </c>
       <c r="J7" s="27">
         <f ca="1">IF(B4&gt;=NOW(),((NOW()-B3)/(B4-B3))*F4,IF(B5&gt;=NOW(),((NOW()-B4)/(B5-B4))*F5,IF(B6&gt;=NOW(),((NOW()-B5)/(B6-B5))*F6,IF(B7&gt;=NOW(),((NOW()-B6)/(B7-B6))*F7,IF(B8&gt;=NOW(),((NOW()-B7)/(B8-B7))*F8,IF(B9&gt;=NOW(),((NOW()-B8)/(B9-B8))*F9,IF(B10&gt;=NOW(),((NOW()-B9)/(B10-B9))*F10,IF(B11&gt;=NOW(),((NOW()-B10)/(B11-B10))*F11,IF(B12&gt;=NOW(),((NOW()-B11)/(B12-B11))*F12,IF(B13&gt;=NOW(),((NOW()-B12)/(B13-B12))*F13,IF(B14&gt;=NOW(),((NOW()-B13)/(B14-B13))*F14,IF(B15&gt;=NOW(),((NOW()-B14)/(B15-B14))*F15,IF(B16&gt;=NOW(),((NOW()-B15)/(B16-B15))*F16,IF(B17&gt;=NOW(),((NOW()-B16)/(B17-B16))*F17,IF(B18&gt;=NOW(),((NOW()-B17)/(B18-B17))*F18,IF(B19&gt;=NOW(),((NOW()-B18)/(B19-B18))*F19,IF(B20&gt;=NOW(),((NOW()-B19)/(B20-B19))*F20,IF(B21&gt;=NOW(),((NOW()-B20)/(B21-B20))*F21,IF(B22&gt;=NOW(),((NOW()-B21)/(B22-B21))*F22,IF(B23&gt;=NOW(),((NOW()-B22)/(B23-B22))*F23,IF(B24&gt;=NOW(),((NOW()-B23)/(B24-B23))*F24,IF(B25&gt;=NOW(),((NOW()-B24)/(B25-B24))*F25,IF(B26&gt;=NOW(),((NOW()-B25)/(B26-B25))*F26,IF(B27&gt;=NOW(),((NOW()-B26)/(B27-B26))*F27,IF(B28&gt;=NOW(),((NOW()-B27)/(B28-B27))*F28,IF(B29&gt;=NOW(),((NOW()-B28)/(B29-B28))*F29,IF(B30&gt;=NOW(),((NOW()-B29)/(B30-B29))*F30,IF(B31&gt;=NOW(),((NOW()-B30)/(B31-B30))*F31,IF(B32&gt;=NOW(),((NOW()-B31)/(B32-B31))*F32,IF(B33&gt;=NOW(),((NOW()-B32)/(B33-B32))*F33,IF(B34&gt;=NOW(),((NOW()-B33)/(B34-B33))*F34,IF(B35&gt;=NOW(),((NOW()-B34)/(B35-B34))*F35,IF(B36&gt;=NOW(),((NOW()-B35)/(B36-B35))*F36,IF(B37&gt;=NOW(),((NOW()-B36)/(B37-B36))*F37,IF(B38&gt;=NOW(),((NOW()-B37)/(B38-B37))*F38,IF(B39&gt;=NOW(),((NOW()-B38)/(B39-B38))*F39,IF(B40&gt;=NOW(),((NOW()-B39)/(B40-B39))*F40,IF(B41&gt;=NOW(),((NOW()-B40)/(B41-B40))*F41,IF(B42&gt;=NOW(),((NOW()-B41)/(B42-B41))*F42,IF(B43&gt;=NOW(),((NOW()-B42)/(B43-B42))*F43,IF(B44&gt;=NOW(),((NOW()-B43)/(B44-B43))*F44,"fin")))))))))))))))))))))))))))))))))))))))))</f>
-        <v>6.8832997621537297E-3</v>
+        <v>6.9763938446655597E-3</v>
       </c>
       <c r="L7" s="22"/>
       <c r="S7" s="12"/>
@@ -21631,7 +21638,7 @@
       </c>
       <c r="J11" s="27">
         <f ca="1">IF(NOW()&lt;B4,C4+((NOW()-B3)/(B4-B3))*F4,IF(NOW()&lt;B5,C5+((NOW()-B4)/(B5-B4))*F5+F4,IF(NOW()&lt;B6,C6+((NOW()-B5)/(B6-B5))*F6+SUM(F4:F5),IF(NOW()&lt;B7,C7+((NOW()-B6)/(B7-B6))*F7+SUM(F4:F6),IF(NOW()&lt;B8,C8+((NOW()-B7)/(B8-B7))*F8+SUM(F4:F7),IF(NOW()&lt;B9,C9+((NOW()-B8)/(B9-B8))*F9+SUM(F4:F8),IF(NOW()&lt;B10,C10+((NOW()-B9)/(B10-B9))*F10+SUM(F4:F9),IF(NOW()&lt;B11,C11+((NOW()-B10)/(B11-B10))*F11+SUM(F4:F10),IF(NOW()&lt;B12,C12+((NOW()-B11)/(B12-B11))*F12+SUM(F4:F11),IF(NOW()&lt;B13,C13+((NOW()-B12)/(B13-B12))*F13+SUM(F4:F12),IF(NOW()&lt;B14,C14+((NOW()-B13)/(B14-B13))*F14+SUM(F4:F13),IF(NOW()&lt;B15,C15+((NOW()-B14)/(B15-B14))*F15+SUM(F4:F14),IF(NOW()&lt;B16,C16+((NOW()-B15)/(B16-B15))*F16+SUM(F4:F15),IF(NOW()&lt;B17,C17+((NOW()-B16)/(B17-B16))*F17+SUM(F4:F16),IF(NOW()&lt;B18,C18+((NOW()-B17)/(B18-B17))*F18+SUM(F4:F17),IF(NOW()&lt;B19,C19+((NOW()-B18)/(B19-B18))*F19+SUM(F4:F18),IF(NOW()&lt;B20,C20+((NOW()-B19)/(B20-B19))*F20+SUM(F4:F19),IF(NOW()&lt;B21,C21+((NOW()-B20)/(B21-B20))*F21+SUM(F4:F20),IF(B22&lt;NOW(),C22+((NOW()-B21)/(B22-B21))*F22+SUM(F4:F21),IF(NOW()&lt;B23,C23+((NOW()-B22)/(B23-B22))*F23+SUM(F4:F22),IF(NOW()&lt;B24,C24+((NOW()-B23)/(B24-B23))*F24+SUM(F4:F23),IF(NOW()&lt;B25,C25+((NOW()-B24)/(B25-B24))*F25+SUM(F4:F24),IF(NOW()&lt;B26,C26+((NOW()-B25)/(B26-B25))*F26+SUM(F4:F25),IF(NOW()&lt;B27,C27+((NOW()-B26)/(B27-B26))*F27+SUM(F4:F26),IF(NOW()&lt;B28,C28+((NOW()-B27)/(B28-B27))*F28+SUM(F4:F27),IF(NOW()&lt;B29,C29+((NOW()-B28)/(B29-B28))*F29+SUM(F4:F28),IF(NOW()&lt;B30,C30+((NOW()-B29)/(B30-B29))*F30+SUM(F4:F29),IF(NOW()&lt;B31,C31+((NOW()-B30)/(B31-B30))*F31+SUM(F4:F30),IF(NOW()&lt;B32,C32+((NOW()-B31)/(B32-B31))*F32+SUM(F4:F31),IF(NOW()&lt;B33,C33+((NOW()-B32)/(B33-B32))*F33+SUM(F4:F32),IF(NOW()&lt;B34,C34+((NOW()-B33)/(B34-B33))*F34+SUM(F4:F33),IF(B35&lt;NOW(),C35+((NOW()-B34)/(B35-B34))*F35+SUM(F4:F34),IF(NOW()&lt;B36,C36+((NOW()-B35)/(B36-B35))*F36+SUM(F4:F35),IF(NOW()&lt;B37,C37+((NOW()-B36)/(B37-B36))*F37+SUM(F4:F36),IF(NOW()&lt;B38,C38+((NOW()-B37)/(B38-B37))*F38+SUM(F4:F37),IF(NOW()&lt;B39,C39+((NOW()-B38)/(B39-B38))*F39+SUM(F4:F38),IF(NOW()&lt;B40,C40+((NOW()-B39)/(B40-B39))*F40+SUM(F4:F39),IF(NOW()&lt;B41,C41+((NOW()-B40)/(B41-B40))*F41+SUM(F4:F40),IF(NOW()&lt;B42,C42+((NOW()-B41)/(B42-B41))*F42+SUM(F4:F41),IF(NOW()&lt;B43,C43+((NOW()-B42)/(B43-B42))*F43+SUM(F4:F42),IF(NOW()&lt;B44,C44+((NOW()-B43)/(B44-B43))*F44+SUM(F4:F43),"Fin")))))))))))))))))))))))))))))))))))))))))</f>
-        <v>104.36688329976215</v>
+        <v>104.36697639384467</v>
       </c>
       <c r="L11" s="22"/>
       <c r="S11" s="12"/>
@@ -22844,7 +22851,7 @@
       </c>
       <c r="J6" s="27">
         <f ca="1">IF(B4&gt;=NOW(),((NOW()-B3)/(B4-B3))*F4,IF(B5&gt;=NOW(),((NOW()-B4)/(B5-B4))*F5,IF(B6&gt;=NOW(),((NOW()-B5)/(B6-B5))*F6,IF(B7&gt;=NOW(),((NOW()-B6)/(B7-B6))*F7,IF(B8&gt;=NOW(),((NOW()-B7)/(B8-B7))*F8,IF(B9&gt;=NOW(),((NOW()-B8)/(B9-B8))*F9,IF(B10&gt;=NOW(),((NOW()-B9)/(B10-B9))*F10,IF(B11&gt;=NOW(),((NOW()-B10)/(B11-B10))*F11,IF(B12&gt;=NOW(),((NOW()-B11)/(B12-B11))*F12,IF(B13&gt;=NOW(),((NOW()-B12)/(B13-B12))*F13,IF(B14&gt;=NOW(),((NOW()-B13)/(B14-B13))*F14,IF(B15&gt;=NOW(),((NOW()-B14)/(B15-B14))*F15,IF(B16&gt;=NOW(),((NOW()-B15)/(B16-B15))*F16,IF(B17&gt;=NOW(),((NOW()-B16)/(B17-B16))*F17,IF(B18&gt;=NOW(),((NOW()-B17)/(B18-B17))*F18,IF(B19&gt;=NOW(),((NOW()-B18)/(B19-B18))*F19,IF(B20&gt;=NOW(),((NOW()-B19)/(B20-B19))*F20,"fin")))))))))))))))))</f>
-        <v>1.9666570749010655E-3</v>
+        <v>1.9932553841901599E-3</v>
       </c>
       <c r="L6" s="22"/>
       <c r="M6">
@@ -22974,7 +22981,7 @@
       </c>
       <c r="J10" s="27">
         <f ca="1">IF(NOW()&lt;B4,C4+((NOW()-B3)/(B4-B3))*F4,IF(NOW()&lt;B5,C5+((NOW()-B4)/(B5-B4))*F5+F4,IF(NOW()&lt;B6,C6+((NOW()-B5)/(B6-B5))*F6+SUM(F4:F5),IF(NOW()&lt;B7,C7+((NOW()-B6)/(B7-B6))*F7+SUM(F4:F6),IF(NOW()&lt;B8,C8+((NOW()-B7)/(B8-B7))*F8+SUM(F4:F7),IF(NOW()&lt;B9,C9+((NOW()-B8)/(B9-B8))*F9+SUM(F4:F8),IF(NOW()&lt;B10,C10+((NOW()-B9)/(B10-B9))*F10+SUM(F4:F9),IF(NOW()&lt;B11,C11+((NOW()-B10)/(B11-B10))*F11+SUM(F4:F10),IF(NOW()&lt;B12,C12+((NOW()-B11)/(B12-B11))*F12+SUM(F4:F11),IF(NOW()&lt;B13,C13+((NOW()-B12)/(B13-B12))*F13+SUM(F4:F12),IF(NOW()&lt;B14,C14+((NOW()-B13)/(B14-B13))*F14+SUM(F4:F13),IF(NOW()&lt;B15,C15+((NOW()-B14)/(B15-B14))*F15+SUM(F4:F14),IF(NOW()&lt;B16,C16+((NOW()-B15)/(B16-B15))*F16+SUM(F4:F15),IF(NOW()&lt;B17,C17+((NOW()-B16)/(B17-B16))*F17+SUM(F4:F16),IF(NOW()&lt;B18,C18+((NOW()-B17)/(B18-B17))*F18+SUM(F4:F17),IF(NOW()&lt;B19,C19+((NOW()-B18)/(B19-B18))*F19+SUM(F4:F18),IF(NOW()&lt;B20,C20+((NOW()-B19)/(B20-B19))*F20+SUM(F4:F19),"fin")))))))))))))))))</f>
-        <v>102.3519666570749</v>
+        <v>102.35199325538419</v>
       </c>
       <c r="L10" s="22"/>
       <c r="M10">

</xml_diff>